<commit_message>
comprueba subgrupos por semanas, quita random a selección de grupos
</commit_message>
<xml_diff>
--- a/lista_subgrupos.xlsx
+++ b/lista_subgrupos.xlsx
@@ -751,112 +751,112 @@
     <t>d.tertre@alumnos.upm.es</t>
   </si>
   <si>
+    <t>MI11-A</t>
+  </si>
+  <si>
+    <t>MI11-B</t>
+  </si>
+  <si>
+    <t>MI11-C</t>
+  </si>
+  <si>
+    <t>MI09-A</t>
+  </si>
+  <si>
+    <t>MI09-B</t>
+  </si>
+  <si>
+    <t>MI09-C</t>
+  </si>
+  <si>
+    <t>MI09-D</t>
+  </si>
+  <si>
     <t>MI11-D</t>
   </si>
   <si>
-    <t>MI11-A</t>
-  </si>
-  <si>
-    <t>MI11-B</t>
-  </si>
-  <si>
-    <t>MI11-C</t>
+    <t>JU09-A</t>
+  </si>
+  <si>
+    <t>JU09-B</t>
+  </si>
+  <si>
+    <t>JU09-C</t>
+  </si>
+  <si>
+    <t>JU09-D</t>
   </si>
   <si>
     <t>JU11-A</t>
   </si>
   <si>
-    <t>MI09-A</t>
-  </si>
-  <si>
-    <t>MI09-B</t>
-  </si>
-  <si>
-    <t>JU09-B</t>
-  </si>
-  <si>
-    <t>JU09-C</t>
+    <t>JU11-B</t>
+  </si>
+  <si>
+    <t>JU11-C</t>
   </si>
   <si>
     <t>JU11-D</t>
   </si>
   <si>
+    <t>VI11-A</t>
+  </si>
+  <si>
+    <t>VI11-B</t>
+  </si>
+  <si>
     <t>VI11-C</t>
   </si>
   <si>
-    <t>JU09-A</t>
-  </si>
-  <si>
-    <t>MI09-C</t>
-  </si>
-  <si>
     <t>VI11-D</t>
   </si>
   <si>
-    <t>JU11-C</t>
-  </si>
-  <si>
-    <t>VI11-B</t>
-  </si>
-  <si>
-    <t>MI09-D</t>
-  </si>
-  <si>
-    <t>JU09-D</t>
-  </si>
-  <si>
-    <t>VI11-A</t>
-  </si>
-  <si>
-    <t>JU11-B</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
+    <t>MI11-E</t>
+  </si>
+  <si>
+    <t>MI11-G</t>
+  </si>
+  <si>
     <t>MI11-F</t>
   </si>
   <si>
-    <t>MI11-E</t>
-  </si>
-  <si>
-    <t>MI11-G</t>
+    <t>VI09-E</t>
+  </si>
+  <si>
+    <t>JU11-E</t>
+  </si>
+  <si>
+    <t>VI09-B</t>
+  </si>
+  <si>
+    <t>JU11-G</t>
+  </si>
+  <si>
+    <t>VI09-F</t>
   </si>
   <si>
     <t>JU11-F</t>
   </si>
   <si>
-    <t>VI09-F</t>
+    <t>VI09-A</t>
+  </si>
+  <si>
+    <t>VI09-G</t>
+  </si>
+  <si>
+    <t>VI09-D</t>
   </si>
   <si>
     <t>VI09-C</t>
   </si>
   <si>
-    <t>VI09-D</t>
-  </si>
-  <si>
-    <t>VI09-B</t>
-  </si>
-  <si>
-    <t>VI09-G</t>
-  </si>
-  <si>
-    <t>JU11-G</t>
-  </si>
-  <si>
-    <t>VI09-E</t>
-  </si>
-  <si>
-    <t>VI09-A</t>
-  </si>
-  <si>
-    <t>JU11-E</t>
+    <t>MA11-A</t>
   </si>
   <si>
     <t>MA11-B</t>
-  </si>
-  <si>
-    <t>MA11-A</t>
   </si>
   <si>
     <t>MA11-C</t>
@@ -1245,7 +1245,7 @@
         <v>245</v>
       </c>
       <c r="C2" t="s">
-        <v>266</v>
+        <v>246</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1253,7 +1253,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D3" t="s">
         <v>279</v>
@@ -1275,10 +1275,10 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D5" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1286,7 +1286,7 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1294,7 +1294,7 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C7" t="s">
         <v>246</v>
@@ -1305,10 +1305,10 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C8" t="s">
-        <v>267</v>
+        <v>246</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1316,10 +1316,10 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
+        <v>245</v>
+      </c>
+      <c r="C9" t="s">
         <v>246</v>
-      </c>
-      <c r="C9" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1335,10 +1335,10 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
+        <v>246</v>
+      </c>
+      <c r="C11" t="s">
         <v>245</v>
-      </c>
-      <c r="C11" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1349,7 +1349,7 @@
         <v>246</v>
       </c>
       <c r="C12" t="s">
-        <v>266</v>
+        <v>245</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1357,10 +1357,10 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C13" t="s">
-        <v>267</v>
+        <v>247</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1368,10 +1368,10 @@
         <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C14" t="s">
-        <v>266</v>
+        <v>247</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1382,7 +1382,7 @@
         <v>246</v>
       </c>
       <c r="C15" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1393,7 +1393,7 @@
         <v>246</v>
       </c>
       <c r="C16" t="s">
-        <v>267</v>
+        <v>247</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1401,10 +1401,10 @@
         <v>19</v>
       </c>
       <c r="B17" t="s">
+        <v>246</v>
+      </c>
+      <c r="C17" t="s">
         <v>247</v>
-      </c>
-      <c r="C17" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1412,10 +1412,10 @@
         <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="C18" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1423,10 +1423,10 @@
         <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C19" t="s">
-        <v>267</v>
+        <v>245</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1434,10 +1434,10 @@
         <v>22</v>
       </c>
       <c r="B20" t="s">
+        <v>247</v>
+      </c>
+      <c r="C20" t="s">
         <v>245</v>
-      </c>
-      <c r="C20" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1445,10 +1445,10 @@
         <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C21" t="s">
-        <v>267</v>
+        <v>245</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1456,7 +1456,7 @@
         <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="D22" t="s">
         <v>279</v>
@@ -1467,10 +1467,10 @@
         <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C23" t="s">
-        <v>267</v>
+        <v>245</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1489,7 +1489,7 @@
         <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1497,13 +1497,13 @@
         <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C26" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="D26" t="s">
-        <v>257</v>
+        <v>281</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1511,13 +1511,13 @@
         <v>29</v>
       </c>
       <c r="B27" t="s">
+        <v>248</v>
+      </c>
+      <c r="C27" t="s">
+        <v>257</v>
+      </c>
+      <c r="D27" t="s">
         <v>249</v>
-      </c>
-      <c r="C27" t="s">
-        <v>266</v>
-      </c>
-      <c r="D27" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1525,13 +1525,13 @@
         <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C28" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="D28" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1539,7 +1539,7 @@
         <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1547,10 +1547,10 @@
         <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D30" t="s">
-        <v>247</v>
+        <v>280</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1558,13 +1558,13 @@
         <v>33</v>
       </c>
       <c r="B31" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="C31" t="s">
-        <v>249</v>
+        <v>266</v>
       </c>
       <c r="D31" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1572,10 +1572,10 @@
         <v>34</v>
       </c>
       <c r="B32" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="C32" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D32" t="s">
         <v>280</v>
@@ -1586,13 +1586,13 @@
         <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="C33" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="D33" t="s">
-        <v>257</v>
+        <v>280</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1600,13 +1600,13 @@
         <v>36</v>
       </c>
       <c r="B34" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="C34" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="D34" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1614,13 +1614,13 @@
         <v>37</v>
       </c>
       <c r="B35" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="C35" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D35" t="s">
-        <v>279</v>
+        <v>248</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1631,10 +1631,10 @@
         <v>249</v>
       </c>
       <c r="C36" t="s">
-        <v>264</v>
+        <v>247</v>
       </c>
       <c r="D36" t="s">
-        <v>246</v>
+        <v>281</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1642,10 +1642,10 @@
         <v>39</v>
       </c>
       <c r="B37" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C37" t="s">
-        <v>271</v>
+        <v>252</v>
       </c>
       <c r="D37" t="s">
         <v>280</v>
@@ -1656,7 +1656,7 @@
         <v>40</v>
       </c>
       <c r="B38" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1664,13 +1664,13 @@
         <v>41</v>
       </c>
       <c r="B39" t="s">
+        <v>249</v>
+      </c>
+      <c r="C39" t="s">
         <v>252</v>
       </c>
-      <c r="C39" t="s">
-        <v>259</v>
-      </c>
       <c r="D39" t="s">
-        <v>247</v>
+        <v>281</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1678,10 +1678,10 @@
         <v>42</v>
       </c>
       <c r="B40" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="D40" t="s">
-        <v>281</v>
+        <v>248</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1689,7 +1689,7 @@
         <v>43</v>
       </c>
       <c r="B41" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1697,10 +1697,10 @@
         <v>44</v>
       </c>
       <c r="B42" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="C42" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1708,13 +1708,13 @@
         <v>45</v>
       </c>
       <c r="B43" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="C43" t="s">
-        <v>254</v>
+        <v>268</v>
       </c>
       <c r="D43" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1722,7 +1722,7 @@
         <v>46</v>
       </c>
       <c r="B44" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1730,13 +1730,13 @@
         <v>47</v>
       </c>
       <c r="B45" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C45" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D45" t="s">
-        <v>250</v>
+        <v>281</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1747,7 +1747,7 @@
         <v>250</v>
       </c>
       <c r="C46" t="s">
-        <v>270</v>
+        <v>247</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1755,10 +1755,10 @@
         <v>49</v>
       </c>
       <c r="B47" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="C47" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1766,10 +1766,10 @@
         <v>50</v>
       </c>
       <c r="B48" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C48" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1777,13 +1777,13 @@
         <v>51</v>
       </c>
       <c r="B49" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C49" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D49" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1791,10 +1791,10 @@
         <v>52</v>
       </c>
       <c r="B50" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D50" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1802,10 +1802,10 @@
         <v>53</v>
       </c>
       <c r="B51" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C51" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1813,10 +1813,10 @@
         <v>54</v>
       </c>
       <c r="B52" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="C52" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1824,10 +1824,10 @@
         <v>55</v>
       </c>
       <c r="B53" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="C53" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="D53" t="s">
         <v>281</v>
@@ -1838,10 +1838,10 @@
         <v>56</v>
       </c>
       <c r="B54" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C54" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1849,10 +1849,10 @@
         <v>57</v>
       </c>
       <c r="B55" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D55" t="s">
-        <v>246</v>
+        <v>280</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -1860,10 +1860,10 @@
         <v>58</v>
       </c>
       <c r="B56" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="D56" t="s">
-        <v>246</v>
+        <v>281</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1871,13 +1871,13 @@
         <v>59</v>
       </c>
       <c r="B57" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C57" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D57" t="s">
-        <v>247</v>
+        <v>280</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -1885,13 +1885,13 @@
         <v>60</v>
       </c>
       <c r="B58" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C58" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D58" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -1899,10 +1899,10 @@
         <v>61</v>
       </c>
       <c r="B59" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C59" t="s">
-        <v>246</v>
+        <v>268</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -1910,10 +1910,10 @@
         <v>62</v>
       </c>
       <c r="B60" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C60" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -1921,13 +1921,13 @@
         <v>63</v>
       </c>
       <c r="B61" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C61" t="s">
-        <v>249</v>
+        <v>260</v>
       </c>
       <c r="D61" t="s">
-        <v>248</v>
+        <v>280</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -1935,10 +1935,10 @@
         <v>64</v>
       </c>
       <c r="B62" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="D62" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -1946,10 +1946,10 @@
         <v>65</v>
       </c>
       <c r="B63" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="C63" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -1957,10 +1957,10 @@
         <v>66</v>
       </c>
       <c r="B64" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C64" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="D64" t="s">
         <v>280</v>
@@ -1971,13 +1971,13 @@
         <v>67</v>
       </c>
       <c r="B65" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="C65" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="D65" t="s">
-        <v>251</v>
+        <v>281</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -1985,13 +1985,13 @@
         <v>68</v>
       </c>
       <c r="B66" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C66" t="s">
-        <v>246</v>
+        <v>257</v>
       </c>
       <c r="D66" t="s">
-        <v>250</v>
+        <v>280</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -2002,10 +2002,10 @@
         <v>253</v>
       </c>
       <c r="C67" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="D67" t="s">
-        <v>248</v>
+        <v>281</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -2013,13 +2013,13 @@
         <v>70</v>
       </c>
       <c r="B68" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C68" t="s">
-        <v>271</v>
+        <v>258</v>
       </c>
       <c r="D68" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -2027,10 +2027,10 @@
         <v>71</v>
       </c>
       <c r="B69" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C69" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -2038,13 +2038,13 @@
         <v>72</v>
       </c>
       <c r="B70" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C70" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D70" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -2052,13 +2052,13 @@
         <v>73</v>
       </c>
       <c r="B71" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C71" t="s">
-        <v>246</v>
+        <v>266</v>
       </c>
       <c r="D71" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -2066,7 +2066,7 @@
         <v>74</v>
       </c>
       <c r="B72" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -2074,7 +2074,7 @@
         <v>75</v>
       </c>
       <c r="B73" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -2082,10 +2082,10 @@
         <v>76</v>
       </c>
       <c r="B74" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="C74" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -2093,13 +2093,13 @@
         <v>77</v>
       </c>
       <c r="B75" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="C75" t="s">
-        <v>271</v>
+        <v>247</v>
       </c>
       <c r="D75" t="s">
-        <v>246</v>
+        <v>280</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -2107,7 +2107,7 @@
         <v>78</v>
       </c>
       <c r="B76" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -2123,7 +2123,7 @@
         <v>80</v>
       </c>
       <c r="B78" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -2131,13 +2131,13 @@
         <v>81</v>
       </c>
       <c r="B79" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C79" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D79" t="s">
-        <v>280</v>
+        <v>248</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -2145,13 +2145,13 @@
         <v>82</v>
       </c>
       <c r="B80" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C80" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D80" t="s">
-        <v>248</v>
+        <v>280</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -2159,13 +2159,13 @@
         <v>83</v>
       </c>
       <c r="B81" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="C81" t="s">
-        <v>248</v>
+        <v>259</v>
       </c>
       <c r="D81" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -2173,10 +2173,10 @@
         <v>84</v>
       </c>
       <c r="B82" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="C82" t="s">
-        <v>246</v>
+        <v>267</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -2184,13 +2184,13 @@
         <v>85</v>
       </c>
       <c r="B83" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C83" t="s">
-        <v>246</v>
+        <v>258</v>
       </c>
       <c r="D83" t="s">
-        <v>251</v>
+        <v>280</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -2198,13 +2198,13 @@
         <v>86</v>
       </c>
       <c r="B84" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="C84" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D84" t="s">
-        <v>280</v>
+        <v>248</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -2212,13 +2212,13 @@
         <v>87</v>
       </c>
       <c r="B85" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="C85" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D85" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -2226,7 +2226,7 @@
         <v>88</v>
       </c>
       <c r="B86" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -2237,10 +2237,10 @@
         <v>255</v>
       </c>
       <c r="C87" t="s">
-        <v>270</v>
+        <v>252</v>
       </c>
       <c r="D87" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -2248,13 +2248,13 @@
         <v>90</v>
       </c>
       <c r="B88" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C88" t="s">
-        <v>247</v>
+        <v>272</v>
       </c>
       <c r="D88" t="s">
-        <v>280</v>
+        <v>249</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -2262,10 +2262,10 @@
         <v>91</v>
       </c>
       <c r="B89" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C89" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D89" t="s">
         <v>248</v>
@@ -2276,13 +2276,13 @@
         <v>92</v>
       </c>
       <c r="B90" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="C90" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D90" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -2290,13 +2290,13 @@
         <v>93</v>
       </c>
       <c r="B91" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="C91" t="s">
-        <v>247</v>
+        <v>270</v>
       </c>
       <c r="D91" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -2304,10 +2304,10 @@
         <v>94</v>
       </c>
       <c r="B92" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="C92" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -2315,13 +2315,13 @@
         <v>95</v>
       </c>
       <c r="B93" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="C93" t="s">
-        <v>248</v>
+        <v>275</v>
       </c>
       <c r="D93" t="s">
-        <v>281</v>
+        <v>249</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -2329,13 +2329,13 @@
         <v>96</v>
       </c>
       <c r="B94" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="C94" t="s">
-        <v>245</v>
+        <v>275</v>
       </c>
       <c r="D94" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -2343,13 +2343,13 @@
         <v>97</v>
       </c>
       <c r="B95" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C95" t="s">
-        <v>247</v>
+        <v>272</v>
       </c>
       <c r="D95" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -2357,10 +2357,10 @@
         <v>98</v>
       </c>
       <c r="B96" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C96" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -2371,7 +2371,7 @@
         <v>256</v>
       </c>
       <c r="D97" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -2379,10 +2379,10 @@
         <v>100</v>
       </c>
       <c r="B98" t="s">
+        <v>257</v>
+      </c>
+      <c r="C98" t="s">
         <v>258</v>
-      </c>
-      <c r="C98" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -2390,13 +2390,13 @@
         <v>101</v>
       </c>
       <c r="B99" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="C99" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D99" t="s">
-        <v>250</v>
+        <v>280</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -2404,13 +2404,13 @@
         <v>102</v>
       </c>
       <c r="B100" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C100" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
       <c r="D100" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -2426,13 +2426,13 @@
         <v>104</v>
       </c>
       <c r="B102" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C102" t="s">
         <v>274</v>
       </c>
       <c r="D102" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -2440,7 +2440,7 @@
         <v>105</v>
       </c>
       <c r="B103" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D103" t="s">
         <v>248</v>
@@ -2451,13 +2451,13 @@
         <v>106</v>
       </c>
       <c r="B104" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C104" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D104" t="s">
-        <v>281</v>
+        <v>245</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -2465,13 +2465,13 @@
         <v>107</v>
       </c>
       <c r="B105" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C105" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D105" t="s">
-        <v>280</v>
+        <v>248</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -2479,13 +2479,13 @@
         <v>108</v>
       </c>
       <c r="B106" t="s">
-        <v>251</v>
+        <v>258</v>
       </c>
       <c r="C106" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
       <c r="D106" t="s">
-        <v>281</v>
+        <v>245</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -2493,13 +2493,13 @@
         <v>109</v>
       </c>
       <c r="B107" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C107" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="D107" t="s">
-        <v>281</v>
+        <v>250</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -2507,10 +2507,10 @@
         <v>110</v>
       </c>
       <c r="B108" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C108" t="s">
-        <v>247</v>
+        <v>270</v>
       </c>
       <c r="D108" t="s">
         <v>250</v>
@@ -2521,10 +2521,10 @@
         <v>111</v>
       </c>
       <c r="B109" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D109" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -2535,7 +2535,7 @@
         <v>258</v>
       </c>
       <c r="C110" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="D110" t="s">
         <v>250</v>
@@ -2546,7 +2546,7 @@
         <v>113</v>
       </c>
       <c r="B111" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -2565,7 +2565,7 @@
         <v>115</v>
       </c>
       <c r="B113" t="s">
-        <v>251</v>
+        <v>258</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -2573,13 +2573,13 @@
         <v>116</v>
       </c>
       <c r="B114" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C114" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="D114" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -2587,13 +2587,13 @@
         <v>117</v>
       </c>
       <c r="B115" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="C115" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D115" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -2601,13 +2601,13 @@
         <v>118</v>
       </c>
       <c r="B116" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C116" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D116" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -2615,13 +2615,13 @@
         <v>119</v>
       </c>
       <c r="B117" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
       <c r="C117" t="s">
-        <v>249</v>
+        <v>267</v>
       </c>
       <c r="D117" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -2632,10 +2632,10 @@
         <v>259</v>
       </c>
       <c r="C118" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="D118" t="s">
-        <v>280</v>
+        <v>249</v>
       </c>
     </row>
     <row r="119" spans="1:4">
@@ -2643,13 +2643,13 @@
         <v>121</v>
       </c>
       <c r="B119" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C119" t="s">
-        <v>247</v>
+        <v>258</v>
       </c>
       <c r="D119" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -2657,10 +2657,10 @@
         <v>122</v>
       </c>
       <c r="B120" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
       <c r="C120" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D120" t="s">
         <v>250</v>
@@ -2671,13 +2671,13 @@
         <v>123</v>
       </c>
       <c r="B121" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C121" t="s">
         <v>278</v>
       </c>
       <c r="D121" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -2685,10 +2685,10 @@
         <v>124</v>
       </c>
       <c r="B122" t="s">
+        <v>260</v>
+      </c>
+      <c r="C122" t="s">
         <v>257</v>
-      </c>
-      <c r="C122" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="123" spans="1:4">
@@ -2696,7 +2696,7 @@
         <v>125</v>
       </c>
       <c r="B123" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="124" spans="1:4">
@@ -2707,10 +2707,10 @@
         <v>260</v>
       </c>
       <c r="C124" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="D124" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -2718,7 +2718,7 @@
         <v>127</v>
       </c>
       <c r="B125" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="126" spans="1:4">
@@ -2729,10 +2729,10 @@
         <v>260</v>
       </c>
       <c r="C126" t="s">
-        <v>245</v>
+        <v>270</v>
       </c>
       <c r="D126" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="127" spans="1:4">
@@ -2740,13 +2740,13 @@
         <v>129</v>
       </c>
       <c r="B127" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="C127" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D127" t="s">
-        <v>281</v>
+        <v>249</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -2754,13 +2754,13 @@
         <v>130</v>
       </c>
       <c r="B128" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C128" t="s">
-        <v>247</v>
+        <v>272</v>
       </c>
       <c r="D128" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
     </row>
     <row r="129" spans="1:4">
@@ -2768,10 +2768,10 @@
         <v>131</v>
       </c>
       <c r="B129" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="C129" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -2782,7 +2782,7 @@
         <v>261</v>
       </c>
       <c r="C130" t="s">
-        <v>268</v>
+        <v>278</v>
       </c>
     </row>
     <row r="131" spans="1:4">
@@ -2790,10 +2790,10 @@
         <v>133</v>
       </c>
       <c r="B131" t="s">
-        <v>248</v>
+        <v>261</v>
       </c>
       <c r="C131" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="132" spans="1:4">
@@ -2801,13 +2801,13 @@
         <v>134</v>
       </c>
       <c r="B132" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C132" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D132" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
     </row>
     <row r="133" spans="1:4">
@@ -2823,10 +2823,10 @@
         <v>136</v>
       </c>
       <c r="B134" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D134" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -2834,13 +2834,13 @@
         <v>137</v>
       </c>
       <c r="B135" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C135" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D135" t="s">
-        <v>280</v>
+        <v>250</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -2848,10 +2848,10 @@
         <v>138</v>
       </c>
       <c r="B136" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D136" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -2859,13 +2859,13 @@
         <v>139</v>
       </c>
       <c r="B137" t="s">
-        <v>248</v>
+        <v>261</v>
       </c>
       <c r="C137" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="D137" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -2876,10 +2876,10 @@
         <v>262</v>
       </c>
       <c r="C138" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D138" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="139" spans="1:4">
@@ -2887,13 +2887,13 @@
         <v>141</v>
       </c>
       <c r="B139" t="s">
-        <v>248</v>
+        <v>262</v>
       </c>
       <c r="C139" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="D139" t="s">
-        <v>279</v>
+        <v>249</v>
       </c>
     </row>
     <row r="140" spans="1:4">
@@ -2904,10 +2904,10 @@
         <v>262</v>
       </c>
       <c r="C140" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D140" t="s">
-        <v>281</v>
+        <v>245</v>
       </c>
     </row>
     <row r="141" spans="1:4">
@@ -2915,13 +2915,13 @@
         <v>143</v>
       </c>
       <c r="B141" t="s">
-        <v>248</v>
+        <v>262</v>
       </c>
       <c r="C141" t="s">
         <v>278</v>
       </c>
       <c r="D141" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="142" spans="1:4">
@@ -2932,7 +2932,7 @@
         <v>262</v>
       </c>
       <c r="C142" t="s">
-        <v>248</v>
+        <v>272</v>
       </c>
       <c r="D142" t="s">
         <v>250</v>
@@ -2946,10 +2946,10 @@
         <v>262</v>
       </c>
       <c r="C143" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D143" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="144" spans="1:4">
@@ -2960,10 +2960,10 @@
         <v>262</v>
       </c>
       <c r="C144" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D144" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="145" spans="1:4">
@@ -2974,10 +2974,10 @@
         <v>262</v>
       </c>
       <c r="C145" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D145" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="146" spans="1:4">
@@ -2988,10 +2988,10 @@
         <v>263</v>
       </c>
       <c r="C146" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D146" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
     </row>
     <row r="147" spans="1:4">
@@ -2999,7 +2999,7 @@
         <v>149</v>
       </c>
       <c r="B147" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="148" spans="1:4">
@@ -3010,10 +3010,10 @@
         <v>263</v>
       </c>
       <c r="C148" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
       <c r="D148" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
     </row>
     <row r="149" spans="1:4">
@@ -3021,13 +3021,13 @@
         <v>151</v>
       </c>
       <c r="B149" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C149" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
       <c r="D149" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="150" spans="1:4">
@@ -3038,10 +3038,10 @@
         <v>263</v>
       </c>
       <c r="C150" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="D150" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="151" spans="1:4">
@@ -3049,13 +3049,13 @@
         <v>153</v>
       </c>
       <c r="B151" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C151" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D151" t="s">
-        <v>281</v>
+        <v>246</v>
       </c>
     </row>
     <row r="152" spans="1:4">
@@ -3066,10 +3066,10 @@
         <v>263</v>
       </c>
       <c r="C152" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D152" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="153" spans="1:4">
@@ -3077,10 +3077,10 @@
         <v>155</v>
       </c>
       <c r="B153" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C153" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="154" spans="1:4">
@@ -3088,10 +3088,10 @@
         <v>156</v>
       </c>
       <c r="B154" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D154" t="s">
-        <v>280</v>
+        <v>245</v>
       </c>
     </row>
     <row r="155" spans="1:4">
@@ -3107,7 +3107,7 @@
         <v>158</v>
       </c>
       <c r="B156" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="157" spans="1:4">
@@ -3123,10 +3123,10 @@
         <v>160</v>
       </c>
       <c r="B158" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C158" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
     </row>
     <row r="159" spans="1:4">
@@ -3137,10 +3137,10 @@
         <v>264</v>
       </c>
       <c r="C159" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="D159" t="s">
-        <v>281</v>
+        <v>249</v>
       </c>
     </row>
     <row r="160" spans="1:4">
@@ -3148,13 +3148,13 @@
         <v>162</v>
       </c>
       <c r="B160" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C160" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="D160" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
     </row>
     <row r="161" spans="1:4">
@@ -3165,7 +3165,7 @@
         <v>264</v>
       </c>
       <c r="C161" t="s">
-        <v>268</v>
+        <v>278</v>
       </c>
     </row>
     <row r="162" spans="1:4">
@@ -3176,10 +3176,10 @@
         <v>265</v>
       </c>
       <c r="C162" t="s">
+        <v>274</v>
+      </c>
+      <c r="D162" t="s">
         <v>248</v>
-      </c>
-      <c r="D162" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="163" spans="1:4">
@@ -3190,10 +3190,10 @@
         <v>265</v>
       </c>
       <c r="C163" t="s">
-        <v>245</v>
+        <v>275</v>
       </c>
       <c r="D163" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="164" spans="1:4">
@@ -3204,7 +3204,7 @@
         <v>265</v>
       </c>
       <c r="C164" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
     </row>
     <row r="165" spans="1:4">
@@ -3215,10 +3215,10 @@
         <v>265</v>
       </c>
       <c r="C165" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D165" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="166" spans="1:4">
@@ -3234,7 +3234,7 @@
         <v>169</v>
       </c>
       <c r="C167" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
     </row>
     <row r="168" spans="1:4">
@@ -3242,7 +3242,7 @@
         <v>170</v>
       </c>
       <c r="C168" t="s">
-        <v>269</v>
+        <v>252</v>
       </c>
     </row>
     <row r="169" spans="1:4">
@@ -3250,7 +3250,7 @@
         <v>171</v>
       </c>
       <c r="C169" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
     </row>
     <row r="170" spans="1:4">
@@ -3258,10 +3258,10 @@
         <v>172</v>
       </c>
       <c r="C170" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="D170" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="171" spans="1:4">
@@ -3277,7 +3277,7 @@
         <v>174</v>
       </c>
       <c r="C172" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="173" spans="1:4">
@@ -3285,7 +3285,7 @@
         <v>175</v>
       </c>
       <c r="C173" t="s">
-        <v>259</v>
+        <v>266</v>
       </c>
     </row>
     <row r="174" spans="1:4">
@@ -3293,7 +3293,7 @@
         <v>176</v>
       </c>
       <c r="C174" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="175" spans="1:4">
@@ -3301,7 +3301,7 @@
         <v>177</v>
       </c>
       <c r="C175" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row r="176" spans="1:4">
@@ -3309,7 +3309,7 @@
         <v>178</v>
       </c>
       <c r="C176" t="s">
-        <v>249</v>
+        <v>268</v>
       </c>
     </row>
     <row r="177" spans="1:4">
@@ -3317,7 +3317,7 @@
         <v>179</v>
       </c>
       <c r="C177" t="s">
-        <v>259</v>
+        <v>268</v>
       </c>
       <c r="D177" t="s">
         <v>281</v>
@@ -3328,7 +3328,7 @@
         <v>180</v>
       </c>
       <c r="C178" t="s">
-        <v>259</v>
+        <v>267</v>
       </c>
     </row>
     <row r="179" spans="1:4">
@@ -3336,7 +3336,7 @@
         <v>181</v>
       </c>
       <c r="C179" t="s">
-        <v>270</v>
+        <v>257</v>
       </c>
       <c r="D179" t="s">
         <v>248</v>
@@ -3347,7 +3347,7 @@
         <v>182</v>
       </c>
       <c r="C180" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
     </row>
     <row r="181" spans="1:4">
@@ -3355,10 +3355,10 @@
         <v>183</v>
       </c>
       <c r="C181" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="D181" t="s">
-        <v>247</v>
+        <v>281</v>
       </c>
     </row>
     <row r="182" spans="1:4">
@@ -3366,10 +3366,10 @@
         <v>184</v>
       </c>
       <c r="C182" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="D182" t="s">
-        <v>257</v>
+        <v>281</v>
       </c>
     </row>
     <row r="183" spans="1:4">
@@ -3377,7 +3377,7 @@
         <v>185</v>
       </c>
       <c r="C183" t="s">
-        <v>249</v>
+        <v>259</v>
       </c>
     </row>
     <row r="184" spans="1:4">
@@ -3393,7 +3393,7 @@
         <v>187</v>
       </c>
       <c r="C185" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
     </row>
     <row r="186" spans="1:4">
@@ -3401,7 +3401,7 @@
         <v>188</v>
       </c>
       <c r="C186" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
     </row>
     <row r="187" spans="1:4">
@@ -3409,7 +3409,7 @@
         <v>189</v>
       </c>
       <c r="C187" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
     </row>
     <row r="188" spans="1:4">
@@ -3417,7 +3417,7 @@
         <v>190</v>
       </c>
       <c r="C188" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D188" t="s">
         <v>281</v>
@@ -3428,7 +3428,7 @@
         <v>191</v>
       </c>
       <c r="C189" t="s">
-        <v>248</v>
+        <v>270</v>
       </c>
     </row>
     <row r="190" spans="1:4">
@@ -3436,7 +3436,7 @@
         <v>192</v>
       </c>
       <c r="C190" t="s">
-        <v>245</v>
+        <v>274</v>
       </c>
     </row>
     <row r="191" spans="1:4">
@@ -3444,7 +3444,7 @@
         <v>193</v>
       </c>
       <c r="C191" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="192" spans="1:4">
@@ -3452,10 +3452,10 @@
         <v>194</v>
       </c>
       <c r="C192" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D192" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
     </row>
     <row r="193" spans="1:4">
@@ -3466,7 +3466,7 @@
         <v>278</v>
       </c>
       <c r="D193" t="s">
-        <v>246</v>
+        <v>280</v>
       </c>
     </row>
     <row r="194" spans="1:4">
@@ -3474,7 +3474,7 @@
         <v>196</v>
       </c>
       <c r="C194" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
     </row>
     <row r="195" spans="1:4">
@@ -3482,10 +3482,10 @@
         <v>197</v>
       </c>
       <c r="C195" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D195" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="196" spans="1:4">
@@ -3493,10 +3493,10 @@
         <v>198</v>
       </c>
       <c r="C196" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D196" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
     </row>
     <row r="197" spans="1:4">
@@ -3504,7 +3504,7 @@
         <v>199</v>
       </c>
       <c r="C197" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="D197" t="s">
         <v>246</v>
@@ -3515,7 +3515,7 @@
         <v>200</v>
       </c>
       <c r="C198" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
     </row>
     <row r="199" spans="1:4">
@@ -3523,10 +3523,10 @@
         <v>201</v>
       </c>
       <c r="C199" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D199" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="200" spans="1:4">
@@ -3534,7 +3534,7 @@
         <v>202</v>
       </c>
       <c r="C200" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
     </row>
     <row r="201" spans="1:4">
@@ -3542,10 +3542,10 @@
         <v>203</v>
       </c>
       <c r="C201" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="D201" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
     </row>
     <row r="202" spans="1:4">
@@ -3553,7 +3553,7 @@
         <v>204</v>
       </c>
       <c r="C202" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="203" spans="1:4">
@@ -3561,7 +3561,7 @@
         <v>205</v>
       </c>
       <c r="C203" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="204" spans="1:4">
@@ -3569,10 +3569,10 @@
         <v>206</v>
       </c>
       <c r="C204" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="D204" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="205" spans="1:4">
@@ -3580,7 +3580,7 @@
         <v>207</v>
       </c>
       <c r="C205" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="206" spans="1:4">
@@ -3588,7 +3588,7 @@
         <v>208</v>
       </c>
       <c r="C206" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="207" spans="1:4">
@@ -3596,7 +3596,7 @@
         <v>209</v>
       </c>
       <c r="C207" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
     </row>
     <row r="208" spans="1:4">
@@ -3620,7 +3620,7 @@
         <v>212</v>
       </c>
       <c r="D210" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="211" spans="1:4">
@@ -3644,7 +3644,7 @@
         <v>215</v>
       </c>
       <c r="D213" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="214" spans="1:4">
@@ -3668,7 +3668,7 @@
         <v>218</v>
       </c>
       <c r="D216" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="217" spans="1:4">
@@ -3708,7 +3708,7 @@
         <v>223</v>
       </c>
       <c r="D221" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="222" spans="1:4">
@@ -3732,7 +3732,7 @@
         <v>226</v>
       </c>
       <c r="D224" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="225" spans="1:4">
@@ -3748,7 +3748,7 @@
         <v>228</v>
       </c>
       <c r="D226" t="s">
-        <v>248</v>
+        <v>280</v>
       </c>
     </row>
     <row r="227" spans="1:4">
@@ -3756,7 +3756,7 @@
         <v>229</v>
       </c>
       <c r="D227" t="s">
-        <v>251</v>
+        <v>280</v>
       </c>
     </row>
     <row r="228" spans="1:4">
@@ -3764,7 +3764,7 @@
         <v>230</v>
       </c>
       <c r="D228" t="s">
-        <v>257</v>
+        <v>280</v>
       </c>
     </row>
     <row r="229" spans="1:4">
@@ -3772,7 +3772,7 @@
         <v>231</v>
       </c>
       <c r="D229" t="s">
-        <v>251</v>
+        <v>281</v>
       </c>
     </row>
     <row r="230" spans="1:4">
@@ -3780,7 +3780,7 @@
         <v>232</v>
       </c>
       <c r="D230" t="s">
-        <v>257</v>
+        <v>281</v>
       </c>
     </row>
     <row r="231" spans="1:4">
@@ -3788,7 +3788,7 @@
         <v>233</v>
       </c>
       <c r="D231" t="s">
-        <v>248</v>
+        <v>281</v>
       </c>
     </row>
     <row r="232" spans="1:4">
@@ -3796,7 +3796,7 @@
         <v>234</v>
       </c>
       <c r="D232" t="s">
-        <v>247</v>
+        <v>281</v>
       </c>
     </row>
     <row r="233" spans="1:4">
@@ -3804,7 +3804,7 @@
         <v>235</v>
       </c>
       <c r="D233" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
     </row>
     <row r="234" spans="1:4">
@@ -3812,7 +3812,7 @@
         <v>236</v>
       </c>
       <c r="D234" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="235" spans="1:4">
@@ -3820,7 +3820,7 @@
         <v>237</v>
       </c>
       <c r="D235" t="s">
-        <v>280</v>
+        <v>250</v>
       </c>
     </row>
     <row r="236" spans="1:4">
@@ -3828,7 +3828,7 @@
         <v>238</v>
       </c>
       <c r="D236" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="237" spans="1:4">
@@ -3836,7 +3836,7 @@
         <v>239</v>
       </c>
       <c r="D237" t="s">
-        <v>281</v>
+        <v>250</v>
       </c>
     </row>
     <row r="238" spans="1:4">
@@ -3844,7 +3844,7 @@
         <v>240</v>
       </c>
       <c r="D238" t="s">
-        <v>280</v>
+        <v>250</v>
       </c>
     </row>
     <row r="239" spans="1:4">
@@ -3852,7 +3852,7 @@
         <v>241</v>
       </c>
       <c r="D239" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
     </row>
     <row r="240" spans="1:4">
@@ -3860,7 +3860,7 @@
         <v>242</v>
       </c>
       <c r="D240" t="s">
-        <v>280</v>
+        <v>245</v>
       </c>
     </row>
     <row r="241" spans="1:4">
@@ -3868,7 +3868,7 @@
         <v>243</v>
       </c>
       <c r="D241" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
     </row>
     <row r="242" spans="1:4">
@@ -3876,7 +3876,7 @@
         <v>244</v>
       </c>
       <c r="D242" t="s">
-        <v>280</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lista subgrupos pasa a ser un deque
</commit_message>
<xml_diff>
--- a/lista_subgrupos.xlsx
+++ b/lista_subgrupos.xlsx
@@ -757,70 +757,91 @@
     <t>MI11-B</t>
   </si>
   <si>
+    <t>MI11-D</t>
+  </si>
+  <si>
     <t>MI11-C</t>
   </si>
   <si>
+    <t>VI11-A</t>
+  </si>
+  <si>
+    <t>JU11-D</t>
+  </si>
+  <si>
+    <t>JU11-C</t>
+  </si>
+  <si>
+    <t>JU11-B</t>
+  </si>
+  <si>
+    <t>JU11-A</t>
+  </si>
+  <si>
+    <t>JU09-D</t>
+  </si>
+  <si>
+    <t>JU09-C</t>
+  </si>
+  <si>
+    <t>JU09-B</t>
+  </si>
+  <si>
+    <t>JU09-A</t>
+  </si>
+  <si>
+    <t>MI09-D</t>
+  </si>
+  <si>
+    <t>MI09-C</t>
+  </si>
+  <si>
+    <t>MI09-B</t>
+  </si>
+  <si>
     <t>MI09-A</t>
   </si>
   <si>
-    <t>MI09-B</t>
-  </si>
-  <si>
-    <t>MI09-C</t>
-  </si>
-  <si>
-    <t>MI09-D</t>
-  </si>
-  <si>
-    <t>MI11-D</t>
-  </si>
-  <si>
-    <t>JU09-A</t>
-  </si>
-  <si>
-    <t>JU09-B</t>
-  </si>
-  <si>
-    <t>JU09-C</t>
-  </si>
-  <si>
-    <t>JU09-D</t>
-  </si>
-  <si>
-    <t>JU11-A</t>
-  </si>
-  <si>
-    <t>JU11-B</t>
-  </si>
-  <si>
-    <t>JU11-C</t>
-  </si>
-  <si>
-    <t>JU11-D</t>
-  </si>
-  <si>
-    <t>VI11-A</t>
+    <t>VI11-D</t>
+  </si>
+  <si>
+    <t>VI11-C</t>
   </si>
   <si>
     <t>VI11-B</t>
   </si>
   <si>
-    <t>VI11-C</t>
-  </si>
-  <si>
-    <t>VI11-D</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
     <t>MI11-E</t>
   </si>
   <si>
+    <t>MI11-F</t>
+  </si>
+  <si>
     <t>MI11-G</t>
   </si>
   <si>
-    <t>MI11-F</t>
+    <t>VI09-G</t>
+  </si>
+  <si>
+    <t>VI09-A</t>
+  </si>
+  <si>
+    <t>VI09-F</t>
+  </si>
+  <si>
+    <t>JU11-F</t>
+  </si>
+  <si>
+    <t>VI09-C</t>
+  </si>
+  <si>
+    <t>JU11-G</t>
+  </si>
+  <si>
+    <t>VI09-B</t>
   </si>
   <si>
     <t>VI09-E</t>
@@ -829,28 +850,7 @@
     <t>JU11-E</t>
   </si>
   <si>
-    <t>VI09-B</t>
-  </si>
-  <si>
-    <t>JU11-G</t>
-  </si>
-  <si>
-    <t>VI09-F</t>
-  </si>
-  <si>
-    <t>JU11-F</t>
-  </si>
-  <si>
-    <t>VI09-A</t>
-  </si>
-  <si>
-    <t>VI09-G</t>
-  </si>
-  <si>
     <t>VI09-D</t>
-  </si>
-  <si>
-    <t>VI09-C</t>
   </si>
   <si>
     <t>MA11-A</t>
@@ -1278,7 +1278,7 @@
         <v>245</v>
       </c>
       <c r="D5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1297,7 +1297,7 @@
         <v>245</v>
       </c>
       <c r="C7" t="s">
-        <v>246</v>
+        <v>266</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1360,7 +1360,7 @@
         <v>246</v>
       </c>
       <c r="C13" t="s">
-        <v>247</v>
+        <v>267</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1371,7 +1371,7 @@
         <v>246</v>
       </c>
       <c r="C14" t="s">
-        <v>247</v>
+        <v>268</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1379,7 +1379,7 @@
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C15" t="s">
         <v>245</v>
@@ -1390,10 +1390,10 @@
         <v>18</v>
       </c>
       <c r="B16" t="s">
+        <v>248</v>
+      </c>
+      <c r="C16" t="s">
         <v>246</v>
-      </c>
-      <c r="C16" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1404,7 +1404,7 @@
         <v>246</v>
       </c>
       <c r="C17" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1412,10 +1412,10 @@
         <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C18" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1423,7 +1423,7 @@
         <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C19" t="s">
         <v>245</v>
@@ -1434,7 +1434,7 @@
         <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C20" t="s">
         <v>245</v>
@@ -1445,7 +1445,7 @@
         <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C21" t="s">
         <v>245</v>
@@ -1456,7 +1456,7 @@
         <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D22" t="s">
         <v>279</v>
@@ -1467,7 +1467,7 @@
         <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C23" t="s">
         <v>245</v>
@@ -1478,7 +1478,7 @@
         <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C24" t="s">
         <v>245</v>
@@ -1489,7 +1489,7 @@
         <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1497,13 +1497,13 @@
         <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C26" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="D26" t="s">
-        <v>281</v>
+        <v>261</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1511,13 +1511,13 @@
         <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C27" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="D27" t="s">
-        <v>249</v>
+        <v>261</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1525,13 +1525,13 @@
         <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C28" t="s">
-        <v>259</v>
+        <v>267</v>
       </c>
       <c r="D28" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1539,7 +1539,7 @@
         <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1547,10 +1547,10 @@
         <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="D30" t="s">
-        <v>280</v>
+        <v>260</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1558,13 +1558,13 @@
         <v>33</v>
       </c>
       <c r="B31" t="s">
+        <v>254</v>
+      </c>
+      <c r="C31" t="s">
+        <v>268</v>
+      </c>
+      <c r="D31" t="s">
         <v>248</v>
-      </c>
-      <c r="C31" t="s">
-        <v>266</v>
-      </c>
-      <c r="D31" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1572,13 +1572,13 @@
         <v>34</v>
       </c>
       <c r="B32" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
       <c r="C32" t="s">
-        <v>257</v>
+        <v>269</v>
       </c>
       <c r="D32" t="s">
-        <v>280</v>
+        <v>245</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1586,13 +1586,13 @@
         <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="C33" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="D33" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1600,13 +1600,13 @@
         <v>36</v>
       </c>
       <c r="B34" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
       <c r="C34" t="s">
-        <v>266</v>
+        <v>250</v>
       </c>
       <c r="D34" t="s">
-        <v>248</v>
+        <v>260</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1614,13 +1614,13 @@
         <v>37</v>
       </c>
       <c r="B35" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C35" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="D35" t="s">
-        <v>248</v>
+        <v>280</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1628,13 +1628,13 @@
         <v>38</v>
       </c>
       <c r="B36" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C36" t="s">
-        <v>247</v>
+        <v>271</v>
       </c>
       <c r="D36" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1642,13 +1642,13 @@
         <v>39</v>
       </c>
       <c r="B37" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C37" t="s">
-        <v>252</v>
+        <v>272</v>
       </c>
       <c r="D37" t="s">
-        <v>280</v>
+        <v>259</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1656,7 +1656,7 @@
         <v>40</v>
       </c>
       <c r="B38" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1664,13 +1664,13 @@
         <v>41</v>
       </c>
       <c r="B39" t="s">
-        <v>249</v>
+        <v>258</v>
       </c>
       <c r="C39" t="s">
-        <v>252</v>
+        <v>270</v>
       </c>
       <c r="D39" t="s">
-        <v>281</v>
+        <v>245</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1678,10 +1678,10 @@
         <v>42</v>
       </c>
       <c r="B40" t="s">
-        <v>249</v>
+        <v>259</v>
       </c>
       <c r="D40" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1689,7 +1689,7 @@
         <v>43</v>
       </c>
       <c r="B41" t="s">
-        <v>249</v>
+        <v>260</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1697,10 +1697,10 @@
         <v>44</v>
       </c>
       <c r="B42" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="C42" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1708,13 +1708,13 @@
         <v>45</v>
       </c>
       <c r="B43" t="s">
-        <v>250</v>
+        <v>262</v>
       </c>
       <c r="C43" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="D43" t="s">
-        <v>281</v>
+        <v>246</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1722,7 +1722,7 @@
         <v>46</v>
       </c>
       <c r="B44" t="s">
-        <v>250</v>
+        <v>263</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1730,10 +1730,10 @@
         <v>47</v>
       </c>
       <c r="B45" t="s">
-        <v>250</v>
+        <v>264</v>
       </c>
       <c r="C45" t="s">
-        <v>252</v>
+        <v>274</v>
       </c>
       <c r="D45" t="s">
         <v>281</v>
@@ -1744,10 +1744,10 @@
         <v>48</v>
       </c>
       <c r="B46" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C46" t="s">
-        <v>247</v>
+        <v>269</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1758,7 +1758,7 @@
         <v>250</v>
       </c>
       <c r="C47" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1766,10 +1766,10 @@
         <v>50</v>
       </c>
       <c r="B48" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C48" t="s">
-        <v>267</v>
+        <v>274</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1777,10 +1777,10 @@
         <v>51</v>
       </c>
       <c r="B49" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C49" t="s">
-        <v>269</v>
+        <v>251</v>
       </c>
       <c r="D49" t="s">
         <v>248</v>
@@ -1791,10 +1791,10 @@
         <v>52</v>
       </c>
       <c r="B50" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="D50" t="s">
-        <v>248</v>
+        <v>261</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1802,7 +1802,7 @@
         <v>53</v>
       </c>
       <c r="B51" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="C51" t="s">
         <v>266</v>
@@ -1813,10 +1813,10 @@
         <v>54</v>
       </c>
       <c r="B52" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="C52" t="s">
-        <v>260</v>
+        <v>271</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1824,13 +1824,13 @@
         <v>55</v>
       </c>
       <c r="B53" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="C53" t="s">
+        <v>269</v>
+      </c>
+      <c r="D53" t="s">
         <v>260</v>
-      </c>
-      <c r="D53" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1838,10 +1838,10 @@
         <v>56</v>
       </c>
       <c r="B54" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="C54" t="s">
-        <v>267</v>
+        <v>275</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1849,10 +1849,10 @@
         <v>57</v>
       </c>
       <c r="B55" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="D55" t="s">
-        <v>280</v>
+        <v>245</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -1860,10 +1860,10 @@
         <v>58</v>
       </c>
       <c r="B56" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="D56" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1871,13 +1871,13 @@
         <v>59</v>
       </c>
       <c r="B57" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C57" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D57" t="s">
-        <v>280</v>
+        <v>261</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -1885,13 +1885,13 @@
         <v>60</v>
       </c>
       <c r="B58" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="C58" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="D58" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -1899,10 +1899,10 @@
         <v>61</v>
       </c>
       <c r="B59" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="C59" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -1910,10 +1910,10 @@
         <v>62</v>
       </c>
       <c r="B60" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="C60" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -1921,13 +1921,13 @@
         <v>63</v>
       </c>
       <c r="B61" t="s">
-        <v>252</v>
+        <v>260</v>
       </c>
       <c r="C61" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
       <c r="D61" t="s">
-        <v>280</v>
+        <v>246</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -1935,10 +1935,10 @@
         <v>64</v>
       </c>
       <c r="B62" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="D62" t="s">
-        <v>249</v>
+        <v>259</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -1946,10 +1946,10 @@
         <v>65</v>
       </c>
       <c r="B63" t="s">
-        <v>252</v>
+        <v>262</v>
       </c>
       <c r="C63" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -1957,13 +1957,13 @@
         <v>66</v>
       </c>
       <c r="B64" t="s">
+        <v>263</v>
+      </c>
+      <c r="C64" t="s">
         <v>252</v>
       </c>
-      <c r="C64" t="s">
-        <v>259</v>
-      </c>
       <c r="D64" t="s">
-        <v>280</v>
+        <v>260</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -1971,13 +1971,13 @@
         <v>67</v>
       </c>
       <c r="B65" t="s">
-        <v>252</v>
+        <v>264</v>
       </c>
       <c r="C65" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
       <c r="D65" t="s">
-        <v>281</v>
+        <v>245</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -1985,13 +1985,13 @@
         <v>68</v>
       </c>
       <c r="B66" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C66" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="D66" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -1999,13 +1999,13 @@
         <v>69</v>
       </c>
       <c r="B67" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C67" t="s">
-        <v>252</v>
+        <v>276</v>
       </c>
       <c r="D67" t="s">
-        <v>281</v>
+        <v>248</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -2013,13 +2013,13 @@
         <v>70</v>
       </c>
       <c r="B68" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C68" t="s">
-        <v>258</v>
+        <v>276</v>
       </c>
       <c r="D68" t="s">
-        <v>248</v>
+        <v>281</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -2027,10 +2027,10 @@
         <v>71</v>
       </c>
       <c r="B69" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C69" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -2041,10 +2041,10 @@
         <v>253</v>
       </c>
       <c r="C70" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="D70" t="s">
-        <v>248</v>
+        <v>259</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -2052,13 +2052,13 @@
         <v>73</v>
       </c>
       <c r="B71" t="s">
+        <v>254</v>
+      </c>
+      <c r="C71" t="s">
         <v>253</v>
       </c>
-      <c r="C71" t="s">
-        <v>266</v>
-      </c>
       <c r="D71" t="s">
-        <v>281</v>
+        <v>259</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -2066,7 +2066,7 @@
         <v>74</v>
       </c>
       <c r="B72" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -2074,7 +2074,7 @@
         <v>75</v>
       </c>
       <c r="B73" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -2082,10 +2082,10 @@
         <v>76</v>
       </c>
       <c r="B74" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C74" t="s">
-        <v>266</v>
+        <v>247</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -2093,13 +2093,13 @@
         <v>77</v>
       </c>
       <c r="B75" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C75" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D75" t="s">
-        <v>280</v>
+        <v>248</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -2107,7 +2107,7 @@
         <v>78</v>
       </c>
       <c r="B76" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -2115,7 +2115,7 @@
         <v>79</v>
       </c>
       <c r="B77" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -2123,7 +2123,7 @@
         <v>80</v>
       </c>
       <c r="B78" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -2131,13 +2131,13 @@
         <v>81</v>
       </c>
       <c r="B79" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="C79" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D79" t="s">
-        <v>248</v>
+        <v>280</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -2145,13 +2145,13 @@
         <v>82</v>
       </c>
       <c r="B80" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="C80" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="D80" t="s">
-        <v>280</v>
+        <v>245</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -2159,13 +2159,13 @@
         <v>83</v>
       </c>
       <c r="B81" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="C81" t="s">
-        <v>259</v>
+        <v>268</v>
       </c>
       <c r="D81" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -2173,10 +2173,10 @@
         <v>84</v>
       </c>
       <c r="B82" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="C82" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -2184,13 +2184,13 @@
         <v>85</v>
       </c>
       <c r="B83" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="C83" t="s">
-        <v>258</v>
+        <v>274</v>
       </c>
       <c r="D83" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -2198,13 +2198,13 @@
         <v>86</v>
       </c>
       <c r="B84" t="s">
-        <v>255</v>
+        <v>263</v>
       </c>
       <c r="C84" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="D84" t="s">
-        <v>248</v>
+        <v>281</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -2212,13 +2212,13 @@
         <v>87</v>
       </c>
       <c r="B85" t="s">
-        <v>255</v>
+        <v>264</v>
       </c>
       <c r="C85" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D85" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -2226,7 +2226,7 @@
         <v>88</v>
       </c>
       <c r="B86" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -2234,13 +2234,13 @@
         <v>89</v>
       </c>
       <c r="B87" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="C87" t="s">
-        <v>252</v>
+        <v>277</v>
       </c>
       <c r="D87" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -2248,13 +2248,13 @@
         <v>90</v>
       </c>
       <c r="B88" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C88" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D88" t="s">
-        <v>249</v>
+        <v>260</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -2262,13 +2262,13 @@
         <v>91</v>
       </c>
       <c r="B89" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C89" t="s">
         <v>273</v>
       </c>
       <c r="D89" t="s">
-        <v>248</v>
+        <v>281</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -2276,13 +2276,13 @@
         <v>92</v>
       </c>
       <c r="B90" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C90" t="s">
-        <v>274</v>
+        <v>252</v>
       </c>
       <c r="D90" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -2290,13 +2290,13 @@
         <v>93</v>
       </c>
       <c r="B91" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C91" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="D91" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -2304,10 +2304,10 @@
         <v>94</v>
       </c>
       <c r="B92" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C92" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -2318,10 +2318,10 @@
         <v>256</v>
       </c>
       <c r="C93" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D93" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -2329,13 +2329,13 @@
         <v>96</v>
       </c>
       <c r="B94" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C94" t="s">
-        <v>275</v>
+        <v>252</v>
       </c>
       <c r="D94" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -2346,10 +2346,10 @@
         <v>256</v>
       </c>
       <c r="C95" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="D95" t="s">
-        <v>249</v>
+        <v>280</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -2360,7 +2360,7 @@
         <v>256</v>
       </c>
       <c r="C96" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -2371,7 +2371,7 @@
         <v>256</v>
       </c>
       <c r="D97" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -2379,10 +2379,10 @@
         <v>100</v>
       </c>
       <c r="B98" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C98" t="s">
-        <v>258</v>
+        <v>266</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -2390,13 +2390,13 @@
         <v>101</v>
       </c>
       <c r="B99" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C99" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="D99" t="s">
-        <v>280</v>
+        <v>248</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -2404,13 +2404,13 @@
         <v>102</v>
       </c>
       <c r="B100" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="C100" t="s">
-        <v>274</v>
+        <v>252</v>
       </c>
       <c r="D100" t="s">
-        <v>249</v>
+        <v>280</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -2418,7 +2418,7 @@
         <v>103</v>
       </c>
       <c r="B101" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -2426,13 +2426,13 @@
         <v>104</v>
       </c>
       <c r="B102" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="C102" t="s">
-        <v>274</v>
+        <v>251</v>
       </c>
       <c r="D102" t="s">
-        <v>249</v>
+        <v>281</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -2440,10 +2440,10 @@
         <v>105</v>
       </c>
       <c r="B103" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="D103" t="s">
-        <v>248</v>
+        <v>261</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -2451,13 +2451,13 @@
         <v>106</v>
       </c>
       <c r="B104" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="C104" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="D104" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -2465,13 +2465,13 @@
         <v>107</v>
       </c>
       <c r="B105" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
       <c r="C105" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D105" t="s">
-        <v>248</v>
+        <v>280</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -2479,13 +2479,13 @@
         <v>108</v>
       </c>
       <c r="B106" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="C106" t="s">
-        <v>277</v>
+        <v>250</v>
       </c>
       <c r="D106" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -2493,13 +2493,13 @@
         <v>109</v>
       </c>
       <c r="B107" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="C107" t="s">
-        <v>271</v>
+        <v>253</v>
       </c>
       <c r="D107" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -2507,13 +2507,13 @@
         <v>110</v>
       </c>
       <c r="B108" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="C108" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="D108" t="s">
-        <v>250</v>
+        <v>280</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -2521,10 +2521,10 @@
         <v>111</v>
       </c>
       <c r="B109" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="D109" t="s">
-        <v>249</v>
+        <v>260</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -2532,13 +2532,13 @@
         <v>112</v>
       </c>
       <c r="B110" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="C110" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="D110" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -2546,7 +2546,7 @@
         <v>113</v>
       </c>
       <c r="B111" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -2554,10 +2554,10 @@
         <v>114</v>
       </c>
       <c r="B112" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C112" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -2565,7 +2565,7 @@
         <v>115</v>
       </c>
       <c r="B113" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -2573,13 +2573,13 @@
         <v>116</v>
       </c>
       <c r="B114" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C114" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="D114" t="s">
-        <v>249</v>
+        <v>280</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -2587,13 +2587,13 @@
         <v>117</v>
       </c>
       <c r="B115" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C115" t="s">
-        <v>270</v>
+        <v>278</v>
       </c>
       <c r="D115" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -2601,13 +2601,13 @@
         <v>118</v>
       </c>
       <c r="B116" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="C116" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D116" t="s">
-        <v>246</v>
+        <v>260</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -2615,13 +2615,13 @@
         <v>119</v>
       </c>
       <c r="B117" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="C117" t="s">
-        <v>267</v>
+        <v>251</v>
       </c>
       <c r="D117" t="s">
-        <v>250</v>
+        <v>280</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -2629,13 +2629,13 @@
         <v>120</v>
       </c>
       <c r="B118" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="C118" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D118" t="s">
-        <v>249</v>
+        <v>261</v>
       </c>
     </row>
     <row r="119" spans="1:4">
@@ -2643,13 +2643,13 @@
         <v>121</v>
       </c>
       <c r="B119" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C119" t="s">
-        <v>258</v>
+        <v>275</v>
       </c>
       <c r="D119" t="s">
-        <v>245</v>
+        <v>281</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -2660,10 +2660,10 @@
         <v>259</v>
       </c>
       <c r="C120" t="s">
-        <v>277</v>
+        <v>253</v>
       </c>
       <c r="D120" t="s">
-        <v>250</v>
+        <v>260</v>
       </c>
     </row>
     <row r="121" spans="1:4">
@@ -2671,13 +2671,13 @@
         <v>123</v>
       </c>
       <c r="B121" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C121" t="s">
         <v>278</v>
       </c>
       <c r="D121" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -2685,10 +2685,10 @@
         <v>124</v>
       </c>
       <c r="B122" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C122" t="s">
-        <v>257</v>
+        <v>268</v>
       </c>
     </row>
     <row r="123" spans="1:4">
@@ -2696,7 +2696,7 @@
         <v>125</v>
       </c>
       <c r="B123" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="124" spans="1:4">
@@ -2704,13 +2704,13 @@
         <v>126</v>
       </c>
       <c r="B124" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="C124" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D124" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -2718,7 +2718,7 @@
         <v>127</v>
       </c>
       <c r="B125" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
     </row>
     <row r="126" spans="1:4">
@@ -2726,13 +2726,13 @@
         <v>128</v>
       </c>
       <c r="B126" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="C126" t="s">
-        <v>270</v>
+        <v>277</v>
       </c>
       <c r="D126" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
     </row>
     <row r="127" spans="1:4">
@@ -2740,13 +2740,13 @@
         <v>129</v>
       </c>
       <c r="B127" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="C127" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="D127" t="s">
-        <v>249</v>
+        <v>280</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -2754,13 +2754,13 @@
         <v>130</v>
       </c>
       <c r="B128" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="C128" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="D128" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="129" spans="1:4">
@@ -2768,10 +2768,10 @@
         <v>131</v>
       </c>
       <c r="B129" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="C129" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -2779,10 +2779,10 @@
         <v>132</v>
       </c>
       <c r="B130" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="C130" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
     </row>
     <row r="131" spans="1:4">
@@ -2790,10 +2790,10 @@
         <v>133</v>
       </c>
       <c r="B131" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="C131" t="s">
-        <v>269</v>
+        <v>278</v>
       </c>
     </row>
     <row r="132" spans="1:4">
@@ -2801,13 +2801,13 @@
         <v>134</v>
       </c>
       <c r="B132" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="C132" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="D132" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="133" spans="1:4">
@@ -2815,7 +2815,7 @@
         <v>135</v>
       </c>
       <c r="B133" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -2823,10 +2823,10 @@
         <v>136</v>
       </c>
       <c r="B134" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="D134" t="s">
-        <v>245</v>
+        <v>281</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -2834,13 +2834,13 @@
         <v>137</v>
       </c>
       <c r="B135" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="C135" t="s">
-        <v>277</v>
+        <v>250</v>
       </c>
       <c r="D135" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -2848,10 +2848,10 @@
         <v>138</v>
       </c>
       <c r="B136" t="s">
+        <v>251</v>
+      </c>
+      <c r="D136" t="s">
         <v>261</v>
-      </c>
-      <c r="D136" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -2859,13 +2859,13 @@
         <v>139</v>
       </c>
       <c r="B137" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
       <c r="C137" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="D137" t="s">
-        <v>245</v>
+        <v>281</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -2873,13 +2873,13 @@
         <v>140</v>
       </c>
       <c r="B138" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
       <c r="C138" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D138" t="s">
-        <v>248</v>
+        <v>259</v>
       </c>
     </row>
     <row r="139" spans="1:4">
@@ -2887,13 +2887,13 @@
         <v>141</v>
       </c>
       <c r="B139" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C139" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="D139" t="s">
-        <v>249</v>
+        <v>259</v>
       </c>
     </row>
     <row r="140" spans="1:4">
@@ -2901,10 +2901,10 @@
         <v>142</v>
       </c>
       <c r="B140" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C140" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D140" t="s">
         <v>245</v>
@@ -2915,13 +2915,13 @@
         <v>143</v>
       </c>
       <c r="B141" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C141" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D141" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
     </row>
     <row r="142" spans="1:4">
@@ -2929,13 +2929,13 @@
         <v>144</v>
       </c>
       <c r="B142" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C142" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D142" t="s">
-        <v>250</v>
+        <v>280</v>
       </c>
     </row>
     <row r="143" spans="1:4">
@@ -2946,10 +2946,10 @@
         <v>262</v>
       </c>
       <c r="C143" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="D143" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="144" spans="1:4">
@@ -2957,13 +2957,13 @@
         <v>146</v>
       </c>
       <c r="B144" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C144" t="s">
-        <v>275</v>
+        <v>253</v>
       </c>
       <c r="D144" t="s">
-        <v>248</v>
+        <v>280</v>
       </c>
     </row>
     <row r="145" spans="1:4">
@@ -2971,7 +2971,7 @@
         <v>147</v>
       </c>
       <c r="B145" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="C145" t="s">
         <v>277</v>
@@ -2985,13 +2985,13 @@
         <v>148</v>
       </c>
       <c r="B146" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
       <c r="C146" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="D146" t="s">
-        <v>250</v>
+        <v>281</v>
       </c>
     </row>
     <row r="147" spans="1:4">
@@ -2999,7 +2999,7 @@
         <v>149</v>
       </c>
       <c r="B147" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
     </row>
     <row r="148" spans="1:4">
@@ -3007,13 +3007,13 @@
         <v>150</v>
       </c>
       <c r="B148" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C148" t="s">
-        <v>274</v>
+        <v>247</v>
       </c>
       <c r="D148" t="s">
-        <v>245</v>
+        <v>281</v>
       </c>
     </row>
     <row r="149" spans="1:4">
@@ -3021,13 +3021,13 @@
         <v>151</v>
       </c>
       <c r="B149" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C149" t="s">
-        <v>277</v>
+        <v>253</v>
       </c>
       <c r="D149" t="s">
-        <v>246</v>
+        <v>261</v>
       </c>
     </row>
     <row r="150" spans="1:4">
@@ -3041,7 +3041,7 @@
         <v>270</v>
       </c>
       <c r="D150" t="s">
-        <v>245</v>
+        <v>281</v>
       </c>
     </row>
     <row r="151" spans="1:4">
@@ -3052,7 +3052,7 @@
         <v>263</v>
       </c>
       <c r="C151" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="D151" t="s">
         <v>246</v>
@@ -3063,10 +3063,10 @@
         <v>154</v>
       </c>
       <c r="B152" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C152" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D152" t="s">
         <v>248</v>
@@ -3077,10 +3077,10 @@
         <v>155</v>
       </c>
       <c r="B153" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C153" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
     </row>
     <row r="154" spans="1:4">
@@ -3088,10 +3088,10 @@
         <v>156</v>
       </c>
       <c r="B154" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D154" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
     </row>
     <row r="155" spans="1:4">
@@ -3099,7 +3099,7 @@
         <v>157</v>
       </c>
       <c r="B155" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="156" spans="1:4">
@@ -3107,7 +3107,7 @@
         <v>158</v>
       </c>
       <c r="B156" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="157" spans="1:4">
@@ -3115,7 +3115,7 @@
         <v>159</v>
       </c>
       <c r="B157" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="158" spans="1:4">
@@ -3123,10 +3123,10 @@
         <v>160</v>
       </c>
       <c r="B158" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="C158" t="s">
-        <v>269</v>
+        <v>251</v>
       </c>
     </row>
     <row r="159" spans="1:4">
@@ -3134,13 +3134,13 @@
         <v>161</v>
       </c>
       <c r="B159" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="C159" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D159" t="s">
-        <v>249</v>
+        <v>280</v>
       </c>
     </row>
     <row r="160" spans="1:4">
@@ -3148,13 +3148,13 @@
         <v>162</v>
       </c>
       <c r="B160" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="C160" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D160" t="s">
-        <v>245</v>
+        <v>261</v>
       </c>
     </row>
     <row r="161" spans="1:4">
@@ -3162,10 +3162,10 @@
         <v>163</v>
       </c>
       <c r="B161" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="C161" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
     </row>
     <row r="162" spans="1:4">
@@ -3176,10 +3176,10 @@
         <v>265</v>
       </c>
       <c r="C162" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="D162" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="163" spans="1:4">
@@ -3190,10 +3190,10 @@
         <v>265</v>
       </c>
       <c r="C163" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="D163" t="s">
-        <v>246</v>
+        <v>261</v>
       </c>
     </row>
     <row r="164" spans="1:4">
@@ -3204,7 +3204,7 @@
         <v>265</v>
       </c>
       <c r="C164" t="s">
-        <v>258</v>
+        <v>278</v>
       </c>
     </row>
     <row r="165" spans="1:4">
@@ -3215,10 +3215,10 @@
         <v>265</v>
       </c>
       <c r="C165" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D165" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="166" spans="1:4">
@@ -3234,7 +3234,7 @@
         <v>169</v>
       </c>
       <c r="C167" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="168" spans="1:4">
@@ -3242,7 +3242,7 @@
         <v>170</v>
       </c>
       <c r="C168" t="s">
-        <v>252</v>
+        <v>278</v>
       </c>
     </row>
     <row r="169" spans="1:4">
@@ -3250,7 +3250,7 @@
         <v>171</v>
       </c>
       <c r="C169" t="s">
-        <v>252</v>
+        <v>273</v>
       </c>
     </row>
     <row r="170" spans="1:4">
@@ -3258,7 +3258,7 @@
         <v>172</v>
       </c>
       <c r="C170" t="s">
-        <v>252</v>
+        <v>275</v>
       </c>
       <c r="D170" t="s">
         <v>280</v>
@@ -3269,7 +3269,7 @@
         <v>173</v>
       </c>
       <c r="C171" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
     </row>
     <row r="172" spans="1:4">
@@ -3277,7 +3277,7 @@
         <v>174</v>
       </c>
       <c r="C172" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
     </row>
     <row r="173" spans="1:4">
@@ -3285,7 +3285,7 @@
         <v>175</v>
       </c>
       <c r="C173" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="174" spans="1:4">
@@ -3293,7 +3293,7 @@
         <v>176</v>
       </c>
       <c r="C174" t="s">
-        <v>268</v>
+        <v>248</v>
       </c>
     </row>
     <row r="175" spans="1:4">
@@ -3301,7 +3301,7 @@
         <v>177</v>
       </c>
       <c r="C175" t="s">
-        <v>268</v>
+        <v>248</v>
       </c>
     </row>
     <row r="176" spans="1:4">
@@ -3309,7 +3309,7 @@
         <v>178</v>
       </c>
       <c r="C176" t="s">
-        <v>268</v>
+        <v>276</v>
       </c>
     </row>
     <row r="177" spans="1:4">
@@ -3317,10 +3317,10 @@
         <v>179</v>
       </c>
       <c r="C177" t="s">
-        <v>268</v>
+        <v>278</v>
       </c>
       <c r="D177" t="s">
-        <v>281</v>
+        <v>261</v>
       </c>
     </row>
     <row r="178" spans="1:4">
@@ -3328,7 +3328,7 @@
         <v>180</v>
       </c>
       <c r="C178" t="s">
-        <v>267</v>
+        <v>252</v>
       </c>
     </row>
     <row r="179" spans="1:4">
@@ -3336,10 +3336,10 @@
         <v>181</v>
       </c>
       <c r="C179" t="s">
-        <v>257</v>
+        <v>267</v>
       </c>
       <c r="D179" t="s">
-        <v>248</v>
+        <v>280</v>
       </c>
     </row>
     <row r="180" spans="1:4">
@@ -3347,7 +3347,7 @@
         <v>182</v>
       </c>
       <c r="C180" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
     </row>
     <row r="181" spans="1:4">
@@ -3355,10 +3355,10 @@
         <v>183</v>
       </c>
       <c r="C181" t="s">
-        <v>258</v>
+        <v>271</v>
       </c>
       <c r="D181" t="s">
-        <v>281</v>
+        <v>259</v>
       </c>
     </row>
     <row r="182" spans="1:4">
@@ -3366,10 +3366,10 @@
         <v>184</v>
       </c>
       <c r="C182" t="s">
-        <v>258</v>
+        <v>270</v>
       </c>
       <c r="D182" t="s">
-        <v>281</v>
+        <v>260</v>
       </c>
     </row>
     <row r="183" spans="1:4">
@@ -3377,7 +3377,7 @@
         <v>185</v>
       </c>
       <c r="C183" t="s">
-        <v>259</v>
+        <v>272</v>
       </c>
     </row>
     <row r="184" spans="1:4">
@@ -3385,7 +3385,7 @@
         <v>186</v>
       </c>
       <c r="C184" t="s">
-        <v>259</v>
+        <v>277</v>
       </c>
     </row>
     <row r="185" spans="1:4">
@@ -3393,7 +3393,7 @@
         <v>187</v>
       </c>
       <c r="C185" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
     </row>
     <row r="186" spans="1:4">
@@ -3401,7 +3401,7 @@
         <v>188</v>
       </c>
       <c r="C186" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
     </row>
     <row r="187" spans="1:4">
@@ -3409,7 +3409,7 @@
         <v>189</v>
       </c>
       <c r="C187" t="s">
-        <v>260</v>
+        <v>276</v>
       </c>
     </row>
     <row r="188" spans="1:4">
@@ -3417,10 +3417,10 @@
         <v>190</v>
       </c>
       <c r="C188" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="D188" t="s">
-        <v>281</v>
+        <v>259</v>
       </c>
     </row>
     <row r="189" spans="1:4">
@@ -3428,7 +3428,7 @@
         <v>191</v>
       </c>
       <c r="C189" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
     </row>
     <row r="190" spans="1:4">
@@ -3436,7 +3436,7 @@
         <v>192</v>
       </c>
       <c r="C190" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
     </row>
     <row r="191" spans="1:4">
@@ -3444,7 +3444,7 @@
         <v>193</v>
       </c>
       <c r="C191" t="s">
-        <v>275</v>
+        <v>250</v>
       </c>
     </row>
     <row r="192" spans="1:4">
@@ -3452,10 +3452,10 @@
         <v>194</v>
       </c>
       <c r="C192" t="s">
-        <v>275</v>
+        <v>251</v>
       </c>
       <c r="D192" t="s">
-        <v>250</v>
+        <v>281</v>
       </c>
     </row>
     <row r="193" spans="1:4">
@@ -3463,10 +3463,10 @@
         <v>195</v>
       </c>
       <c r="C193" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D193" t="s">
-        <v>280</v>
+        <v>248</v>
       </c>
     </row>
     <row r="194" spans="1:4">
@@ -3474,7 +3474,7 @@
         <v>196</v>
       </c>
       <c r="C194" t="s">
-        <v>277</v>
+        <v>252</v>
       </c>
     </row>
     <row r="195" spans="1:4">
@@ -3482,10 +3482,10 @@
         <v>197</v>
       </c>
       <c r="C195" t="s">
-        <v>277</v>
+        <v>253</v>
       </c>
       <c r="D195" t="s">
-        <v>248</v>
+        <v>260</v>
       </c>
     </row>
     <row r="196" spans="1:4">
@@ -3493,10 +3493,10 @@
         <v>198</v>
       </c>
       <c r="C196" t="s">
-        <v>277</v>
+        <v>252</v>
       </c>
       <c r="D196" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="197" spans="1:4">
@@ -3504,10 +3504,10 @@
         <v>199</v>
       </c>
       <c r="C197" t="s">
-        <v>269</v>
+        <v>251</v>
       </c>
       <c r="D197" t="s">
-        <v>246</v>
+        <v>261</v>
       </c>
     </row>
     <row r="198" spans="1:4">
@@ -3515,7 +3515,7 @@
         <v>200</v>
       </c>
       <c r="C198" t="s">
-        <v>269</v>
+        <v>250</v>
       </c>
     </row>
     <row r="199" spans="1:4">
@@ -3526,7 +3526,7 @@
         <v>269</v>
       </c>
       <c r="D199" t="s">
-        <v>249</v>
+        <v>281</v>
       </c>
     </row>
     <row r="200" spans="1:4">
@@ -3534,7 +3534,7 @@
         <v>202</v>
       </c>
       <c r="C200" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="201" spans="1:4">
@@ -3542,7 +3542,7 @@
         <v>203</v>
       </c>
       <c r="C201" t="s">
-        <v>269</v>
+        <v>276</v>
       </c>
       <c r="D201" t="s">
         <v>245</v>
@@ -3553,7 +3553,7 @@
         <v>204</v>
       </c>
       <c r="C202" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="203" spans="1:4">
@@ -3561,7 +3561,7 @@
         <v>205</v>
       </c>
       <c r="C203" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
     </row>
     <row r="204" spans="1:4">
@@ -3569,10 +3569,10 @@
         <v>206</v>
       </c>
       <c r="C204" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D204" t="s">
-        <v>249</v>
+        <v>261</v>
       </c>
     </row>
     <row r="205" spans="1:4">
@@ -3580,7 +3580,7 @@
         <v>207</v>
       </c>
       <c r="C205" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="206" spans="1:4">
@@ -3596,7 +3596,7 @@
         <v>209</v>
       </c>
       <c r="C207" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
     </row>
     <row r="208" spans="1:4">
@@ -3644,7 +3644,7 @@
         <v>215</v>
       </c>
       <c r="D213" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="214" spans="1:4">
@@ -3652,7 +3652,7 @@
         <v>216</v>
       </c>
       <c r="D214" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="215" spans="1:4">
@@ -3716,7 +3716,7 @@
         <v>224</v>
       </c>
       <c r="D222" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="223" spans="1:4">
@@ -3724,7 +3724,7 @@
         <v>225</v>
       </c>
       <c r="D223" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="224" spans="1:4">
@@ -3748,7 +3748,7 @@
         <v>228</v>
       </c>
       <c r="D226" t="s">
-        <v>280</v>
+        <v>259</v>
       </c>
     </row>
     <row r="227" spans="1:4">
@@ -3756,7 +3756,7 @@
         <v>229</v>
       </c>
       <c r="D227" t="s">
-        <v>280</v>
+        <v>261</v>
       </c>
     </row>
     <row r="228" spans="1:4">
@@ -3772,7 +3772,7 @@
         <v>231</v>
       </c>
       <c r="D229" t="s">
-        <v>281</v>
+        <v>260</v>
       </c>
     </row>
     <row r="230" spans="1:4">
@@ -3788,7 +3788,7 @@
         <v>233</v>
       </c>
       <c r="D231" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="232" spans="1:4">
@@ -3796,7 +3796,7 @@
         <v>234</v>
       </c>
       <c r="D232" t="s">
-        <v>281</v>
+        <v>246</v>
       </c>
     </row>
     <row r="233" spans="1:4">
@@ -3804,7 +3804,7 @@
         <v>235</v>
       </c>
       <c r="D233" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="234" spans="1:4">
@@ -3812,7 +3812,7 @@
         <v>236</v>
       </c>
       <c r="D234" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
     </row>
     <row r="235" spans="1:4">
@@ -3820,7 +3820,7 @@
         <v>237</v>
       </c>
       <c r="D235" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
     </row>
     <row r="236" spans="1:4">
@@ -3828,7 +3828,7 @@
         <v>238</v>
       </c>
       <c r="D236" t="s">
-        <v>250</v>
+        <v>260</v>
       </c>
     </row>
     <row r="237" spans="1:4">
@@ -3836,7 +3836,7 @@
         <v>239</v>
       </c>
       <c r="D237" t="s">
-        <v>250</v>
+        <v>281</v>
       </c>
     </row>
     <row r="238" spans="1:4">
@@ -3844,7 +3844,7 @@
         <v>240</v>
       </c>
       <c r="D238" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="239" spans="1:4">
@@ -3852,7 +3852,7 @@
         <v>241</v>
       </c>
       <c r="D239" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
     </row>
     <row r="240" spans="1:4">
@@ -3860,7 +3860,7 @@
         <v>242</v>
       </c>
       <c r="D240" t="s">
-        <v>245</v>
+        <v>281</v>
       </c>
     </row>
     <row r="241" spans="1:4">
@@ -3868,7 +3868,7 @@
         <v>243</v>
       </c>
       <c r="D241" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
     </row>
     <row r="242" spans="1:4">
@@ -3876,7 +3876,7 @@
         <v>244</v>
       </c>
       <c r="D242" t="s">
-        <v>246</v>
+        <v>261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrige calculo semanas de subgrupos
Falta por rematar el asignar subgrupo en caso de misma sesion y semana (ver como hacer 2x break o refactorizar)
</commit_message>
<xml_diff>
--- a/lista_subgrupos.xlsx
+++ b/lista_subgrupos.xlsx
@@ -853,10 +853,10 @@
     <t>VI09-D</t>
   </si>
   <si>
+    <t>MA11-B</t>
+  </si>
+  <si>
     <t>MA11-A</t>
-  </si>
-  <si>
-    <t>MA11-B</t>
   </si>
   <si>
     <t>MA11-C</t>
@@ -1256,7 +1256,7 @@
         <v>245</v>
       </c>
       <c r="D3" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1278,7 +1278,7 @@
         <v>245</v>
       </c>
       <c r="D5" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1319,7 +1319,7 @@
         <v>245</v>
       </c>
       <c r="C9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1404,7 +1404,7 @@
         <v>246</v>
       </c>
       <c r="C17" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1415,7 +1415,7 @@
         <v>246</v>
       </c>
       <c r="C18" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1459,7 +1459,7 @@
         <v>248</v>
       </c>
       <c r="D22" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1470,7 +1470,7 @@
         <v>248</v>
       </c>
       <c r="C23" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1531,7 +1531,7 @@
         <v>267</v>
       </c>
       <c r="D28" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1592,7 +1592,7 @@
         <v>253</v>
       </c>
       <c r="D33" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1634,7 +1634,7 @@
         <v>271</v>
       </c>
       <c r="D36" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1852,7 +1852,7 @@
         <v>247</v>
       </c>
       <c r="D55" t="s">
-        <v>245</v>
+        <v>265</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -1863,7 +1863,7 @@
         <v>247</v>
       </c>
       <c r="D56" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1938,7 +1938,7 @@
         <v>261</v>
       </c>
       <c r="D62" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -1949,7 +1949,7 @@
         <v>262</v>
       </c>
       <c r="C63" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -1991,7 +1991,7 @@
         <v>248</v>
       </c>
       <c r="D66" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -2096,10 +2096,10 @@
         <v>257</v>
       </c>
       <c r="C75" t="s">
+        <v>248</v>
+      </c>
+      <c r="D75" t="s">
         <v>246</v>
-      </c>
-      <c r="D75" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -2279,7 +2279,7 @@
         <v>253</v>
       </c>
       <c r="C90" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D90" t="s">
         <v>246</v>
@@ -2349,7 +2349,7 @@
         <v>278</v>
       </c>
       <c r="D95" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -2410,7 +2410,7 @@
         <v>252</v>
       </c>
       <c r="D100" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -2471,7 +2471,7 @@
         <v>266</v>
       </c>
       <c r="D105" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -2513,7 +2513,7 @@
         <v>250</v>
       </c>
       <c r="D108" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -2579,7 +2579,7 @@
         <v>275</v>
       </c>
       <c r="D114" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -2621,7 +2621,7 @@
         <v>251</v>
       </c>
       <c r="D117" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -2649,7 +2649,7 @@
         <v>275</v>
       </c>
       <c r="D119" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -2660,7 +2660,7 @@
         <v>259</v>
       </c>
       <c r="C120" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D120" t="s">
         <v>260</v>
@@ -2746,7 +2746,7 @@
         <v>267</v>
       </c>
       <c r="D127" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -2837,7 +2837,7 @@
         <v>251</v>
       </c>
       <c r="C135" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D135" t="s">
         <v>245</v>
@@ -2935,7 +2935,7 @@
         <v>269</v>
       </c>
       <c r="D142" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="143" spans="1:4">
@@ -2963,7 +2963,7 @@
         <v>253</v>
       </c>
       <c r="D144" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="145" spans="1:4">
@@ -2991,7 +2991,7 @@
         <v>267</v>
       </c>
       <c r="D146" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="147" spans="1:4">
@@ -3027,7 +3027,7 @@
         <v>253</v>
       </c>
       <c r="D149" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
     </row>
     <row r="150" spans="1:4">
@@ -3041,7 +3041,7 @@
         <v>270</v>
       </c>
       <c r="D150" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="151" spans="1:4">
@@ -3140,7 +3140,7 @@
         <v>272</v>
       </c>
       <c r="D159" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="160" spans="1:4">
@@ -3193,7 +3193,7 @@
         <v>277</v>
       </c>
       <c r="D163" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
     </row>
     <row r="164" spans="1:4">
@@ -3261,7 +3261,7 @@
         <v>275</v>
       </c>
       <c r="D170" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="171" spans="1:4">
@@ -3339,7 +3339,7 @@
         <v>267</v>
       </c>
       <c r="D179" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="180" spans="1:4">
@@ -3504,7 +3504,7 @@
         <v>199</v>
       </c>
       <c r="C197" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D197" t="s">
         <v>261</v>
@@ -3604,7 +3604,7 @@
         <v>210</v>
       </c>
       <c r="D208" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="209" spans="1:4">
@@ -3612,7 +3612,7 @@
         <v>211</v>
       </c>
       <c r="D209" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="210" spans="1:4">
@@ -3620,7 +3620,7 @@
         <v>212</v>
       </c>
       <c r="D210" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="211" spans="1:4">
@@ -3628,7 +3628,7 @@
         <v>213</v>
       </c>
       <c r="D211" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="212" spans="1:4">
@@ -3636,7 +3636,7 @@
         <v>214</v>
       </c>
       <c r="D212" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="213" spans="1:4">
@@ -3652,7 +3652,7 @@
         <v>216</v>
       </c>
       <c r="D214" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="215" spans="1:4">
@@ -3660,7 +3660,7 @@
         <v>217</v>
       </c>
       <c r="D215" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="216" spans="1:4">
@@ -3668,7 +3668,7 @@
         <v>218</v>
       </c>
       <c r="D216" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="217" spans="1:4">
@@ -3676,7 +3676,7 @@
         <v>219</v>
       </c>
       <c r="D217" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="218" spans="1:4">
@@ -3684,7 +3684,7 @@
         <v>220</v>
       </c>
       <c r="D218" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="219" spans="1:4">
@@ -3692,7 +3692,7 @@
         <v>221</v>
       </c>
       <c r="D219" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="220" spans="1:4">
@@ -3700,7 +3700,7 @@
         <v>222</v>
       </c>
       <c r="D220" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="221" spans="1:4">
@@ -3708,7 +3708,7 @@
         <v>223</v>
       </c>
       <c r="D221" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="222" spans="1:4">
@@ -3724,7 +3724,7 @@
         <v>225</v>
       </c>
       <c r="D223" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="224" spans="1:4">
@@ -3732,7 +3732,7 @@
         <v>226</v>
       </c>
       <c r="D224" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="225" spans="1:4">
@@ -3740,7 +3740,7 @@
         <v>227</v>
       </c>
       <c r="D225" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="226" spans="1:4">
@@ -3764,7 +3764,7 @@
         <v>230</v>
       </c>
       <c r="D228" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="229" spans="1:4">
@@ -3876,7 +3876,7 @@
         <v>244</v>
       </c>
       <c r="D242" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactoring estudiante sin/con restricciones
</commit_message>
<xml_diff>
--- a/lista_subgrupos.xlsx
+++ b/lista_subgrupos.xlsx
@@ -814,13 +814,16 @@
     <t>-</t>
   </si>
   <si>
+    <t>MI11-F</t>
+  </si>
+  <si>
+    <t>MI11-G</t>
+  </si>
+  <si>
     <t>MI11-E</t>
   </si>
   <si>
-    <t>MI11-F</t>
-  </si>
-  <si>
-    <t>MI11-G</t>
+    <t>VI09-B</t>
   </si>
   <si>
     <t>VI09-G</t>
@@ -841,22 +844,19 @@
     <t>JU11-G</t>
   </si>
   <si>
-    <t>VI09-B</t>
-  </si>
-  <si>
     <t>VI09-E</t>
   </si>
   <si>
+    <t>VI09-D</t>
+  </si>
+  <si>
     <t>JU11-E</t>
   </si>
   <si>
-    <t>VI09-D</t>
+    <t>MA11-A</t>
   </si>
   <si>
     <t>MA11-B</t>
-  </si>
-  <si>
-    <t>MA11-A</t>
   </si>
   <si>
     <t>MA11-C</t>
@@ -1245,7 +1245,7 @@
         <v>245</v>
       </c>
       <c r="C2" t="s">
-        <v>246</v>
+        <v>266</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1256,7 +1256,7 @@
         <v>245</v>
       </c>
       <c r="D3" t="s">
-        <v>265</v>
+        <v>279</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1267,7 +1267,7 @@
         <v>245</v>
       </c>
       <c r="C4" t="s">
-        <v>246</v>
+        <v>266</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1278,7 +1278,7 @@
         <v>245</v>
       </c>
       <c r="D5" t="s">
-        <v>265</v>
+        <v>279</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1297,7 +1297,7 @@
         <v>245</v>
       </c>
       <c r="C7" t="s">
-        <v>266</v>
+        <v>247</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1308,7 +1308,7 @@
         <v>245</v>
       </c>
       <c r="C8" t="s">
-        <v>246</v>
+        <v>266</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1319,7 +1319,7 @@
         <v>245</v>
       </c>
       <c r="C9" t="s">
-        <v>245</v>
+        <v>267</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1338,7 +1338,7 @@
         <v>246</v>
       </c>
       <c r="C11" t="s">
-        <v>245</v>
+        <v>267</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1349,7 +1349,7 @@
         <v>246</v>
       </c>
       <c r="C12" t="s">
-        <v>245</v>
+        <v>267</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1360,7 +1360,7 @@
         <v>246</v>
       </c>
       <c r="C13" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1371,7 +1371,7 @@
         <v>246</v>
       </c>
       <c r="C14" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1382,7 +1382,7 @@
         <v>247</v>
       </c>
       <c r="C15" t="s">
-        <v>245</v>
+        <v>267</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1393,7 +1393,7 @@
         <v>248</v>
       </c>
       <c r="C16" t="s">
-        <v>246</v>
+        <v>266</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1404,7 +1404,7 @@
         <v>246</v>
       </c>
       <c r="C17" t="s">
-        <v>246</v>
+        <v>266</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1415,7 +1415,7 @@
         <v>246</v>
       </c>
       <c r="C18" t="s">
-        <v>246</v>
+        <v>266</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1426,7 +1426,7 @@
         <v>246</v>
       </c>
       <c r="C19" t="s">
-        <v>245</v>
+        <v>267</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1437,7 +1437,7 @@
         <v>248</v>
       </c>
       <c r="C20" t="s">
-        <v>245</v>
+        <v>267</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1448,7 +1448,7 @@
         <v>248</v>
       </c>
       <c r="C21" t="s">
-        <v>245</v>
+        <v>267</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1459,7 +1459,7 @@
         <v>248</v>
       </c>
       <c r="D22" t="s">
-        <v>265</v>
+        <v>279</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1470,7 +1470,7 @@
         <v>248</v>
       </c>
       <c r="C23" t="s">
-        <v>246</v>
+        <v>266</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1481,7 +1481,7 @@
         <v>248</v>
       </c>
       <c r="C24" t="s">
-        <v>245</v>
+        <v>267</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1500,7 +1500,7 @@
         <v>249</v>
       </c>
       <c r="C26" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="D26" t="s">
         <v>261</v>
@@ -1528,10 +1528,10 @@
         <v>251</v>
       </c>
       <c r="C28" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="D28" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1561,7 +1561,7 @@
         <v>254</v>
       </c>
       <c r="C31" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
       <c r="D31" t="s">
         <v>248</v>
@@ -1575,7 +1575,7 @@
         <v>255</v>
       </c>
       <c r="C32" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D32" t="s">
         <v>245</v>
@@ -1592,7 +1592,7 @@
         <v>253</v>
       </c>
       <c r="D33" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1617,7 +1617,7 @@
         <v>247</v>
       </c>
       <c r="C35" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D35" t="s">
         <v>280</v>
@@ -1631,10 +1631,10 @@
         <v>248</v>
       </c>
       <c r="C36" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D36" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1645,7 +1645,7 @@
         <v>247</v>
       </c>
       <c r="C37" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D37" t="s">
         <v>259</v>
@@ -1667,7 +1667,7 @@
         <v>258</v>
       </c>
       <c r="C39" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D39" t="s">
         <v>245</v>
@@ -1700,7 +1700,7 @@
         <v>261</v>
       </c>
       <c r="C42" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1711,7 +1711,7 @@
         <v>262</v>
       </c>
       <c r="C43" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D43" t="s">
         <v>246</v>
@@ -1733,7 +1733,7 @@
         <v>264</v>
       </c>
       <c r="C45" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D45" t="s">
         <v>281</v>
@@ -1747,7 +1747,7 @@
         <v>249</v>
       </c>
       <c r="C46" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1758,7 +1758,7 @@
         <v>250</v>
       </c>
       <c r="C47" t="s">
-        <v>251</v>
+        <v>271</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1769,7 +1769,7 @@
         <v>251</v>
       </c>
       <c r="C48" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1780,10 +1780,10 @@
         <v>252</v>
       </c>
       <c r="C49" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="D49" t="s">
-        <v>248</v>
+        <v>280</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1805,7 +1805,7 @@
         <v>254</v>
       </c>
       <c r="C51" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1816,7 +1816,7 @@
         <v>255</v>
       </c>
       <c r="C52" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1827,7 +1827,7 @@
         <v>256</v>
       </c>
       <c r="C53" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D53" t="s">
         <v>260</v>
@@ -1841,7 +1841,7 @@
         <v>257</v>
       </c>
       <c r="C54" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1852,7 +1852,7 @@
         <v>247</v>
       </c>
       <c r="D55" t="s">
-        <v>265</v>
+        <v>279</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -1874,7 +1874,7 @@
         <v>247</v>
       </c>
       <c r="C57" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D57" t="s">
         <v>261</v>
@@ -1888,10 +1888,10 @@
         <v>247</v>
       </c>
       <c r="C58" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D58" t="s">
-        <v>246</v>
+        <v>280</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -1902,7 +1902,7 @@
         <v>258</v>
       </c>
       <c r="C59" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -1927,7 +1927,7 @@
         <v>247</v>
       </c>
       <c r="D61" t="s">
-        <v>246</v>
+        <v>280</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -1938,7 +1938,7 @@
         <v>261</v>
       </c>
       <c r="D62" t="s">
-        <v>265</v>
+        <v>245</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -1949,7 +1949,7 @@
         <v>262</v>
       </c>
       <c r="C63" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -1974,7 +1974,7 @@
         <v>264</v>
       </c>
       <c r="C65" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D65" t="s">
         <v>245</v>
@@ -1988,7 +1988,7 @@
         <v>249</v>
       </c>
       <c r="C66" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D66" t="s">
         <v>280</v>
@@ -2030,7 +2030,7 @@
         <v>252</v>
       </c>
       <c r="C69" t="s">
-        <v>250</v>
+        <v>271</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -2041,7 +2041,7 @@
         <v>253</v>
       </c>
       <c r="C70" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="D70" t="s">
         <v>259</v>
@@ -2096,10 +2096,10 @@
         <v>257</v>
       </c>
       <c r="C75" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D75" t="s">
-        <v>246</v>
+        <v>279</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -2162,7 +2162,7 @@
         <v>260</v>
       </c>
       <c r="C81" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
       <c r="D81" t="s">
         <v>281</v>
@@ -2187,7 +2187,7 @@
         <v>262</v>
       </c>
       <c r="C83" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D83" t="s">
         <v>281</v>
@@ -2201,7 +2201,7 @@
         <v>263</v>
       </c>
       <c r="C84" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D84" t="s">
         <v>281</v>
@@ -2215,10 +2215,10 @@
         <v>264</v>
       </c>
       <c r="C85" t="s">
-        <v>268</v>
+        <v>248</v>
       </c>
       <c r="D85" t="s">
-        <v>248</v>
+        <v>260</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -2237,7 +2237,7 @@
         <v>250</v>
       </c>
       <c r="C87" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="D87" t="s">
         <v>248</v>
@@ -2251,7 +2251,7 @@
         <v>251</v>
       </c>
       <c r="C88" t="s">
-        <v>266</v>
+        <v>246</v>
       </c>
       <c r="D88" t="s">
         <v>260</v>
@@ -2265,7 +2265,7 @@
         <v>252</v>
       </c>
       <c r="C89" t="s">
-        <v>273</v>
+        <v>246</v>
       </c>
       <c r="D89" t="s">
         <v>281</v>
@@ -2279,7 +2279,7 @@
         <v>253</v>
       </c>
       <c r="C90" t="s">
-        <v>253</v>
+        <v>269</v>
       </c>
       <c r="D90" t="s">
         <v>246</v>
@@ -2293,7 +2293,7 @@
         <v>254</v>
       </c>
       <c r="C91" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="D91" t="s">
         <v>260</v>
@@ -2307,7 +2307,7 @@
         <v>255</v>
       </c>
       <c r="C92" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -2318,7 +2318,7 @@
         <v>256</v>
       </c>
       <c r="C93" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D93" t="s">
         <v>248</v>
@@ -2346,10 +2346,10 @@
         <v>256</v>
       </c>
       <c r="C95" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D95" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -2360,7 +2360,7 @@
         <v>256</v>
       </c>
       <c r="C96" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -2382,7 +2382,7 @@
         <v>256</v>
       </c>
       <c r="C98" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -2393,7 +2393,7 @@
         <v>258</v>
       </c>
       <c r="C99" t="s">
-        <v>270</v>
+        <v>278</v>
       </c>
       <c r="D99" t="s">
         <v>248</v>
@@ -2410,7 +2410,7 @@
         <v>252</v>
       </c>
       <c r="D100" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -2454,7 +2454,7 @@
         <v>263</v>
       </c>
       <c r="C104" t="s">
-        <v>267</v>
+        <v>247</v>
       </c>
       <c r="D104" t="s">
         <v>259</v>
@@ -2468,10 +2468,10 @@
         <v>264</v>
       </c>
       <c r="C105" t="s">
-        <v>266</v>
+        <v>245</v>
       </c>
       <c r="D105" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -2496,7 +2496,7 @@
         <v>250</v>
       </c>
       <c r="C107" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="D107" t="s">
         <v>261</v>
@@ -2510,10 +2510,10 @@
         <v>251</v>
       </c>
       <c r="C108" t="s">
-        <v>250</v>
+        <v>269</v>
       </c>
       <c r="D108" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -2535,7 +2535,7 @@
         <v>253</v>
       </c>
       <c r="C110" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="D110" t="s">
         <v>248</v>
@@ -2557,7 +2557,7 @@
         <v>255</v>
       </c>
       <c r="C112" t="s">
-        <v>266</v>
+        <v>248</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -2576,10 +2576,10 @@
         <v>255</v>
       </c>
       <c r="C114" t="s">
-        <v>275</v>
+        <v>248</v>
       </c>
       <c r="D114" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -2590,7 +2590,7 @@
         <v>255</v>
       </c>
       <c r="C115" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D115" t="s">
         <v>245</v>
@@ -2604,7 +2604,7 @@
         <v>254</v>
       </c>
       <c r="C116" t="s">
-        <v>268</v>
+        <v>251</v>
       </c>
       <c r="D116" t="s">
         <v>260</v>
@@ -2621,7 +2621,7 @@
         <v>251</v>
       </c>
       <c r="D117" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -2632,7 +2632,7 @@
         <v>254</v>
       </c>
       <c r="C118" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
       <c r="D118" t="s">
         <v>261</v>
@@ -2646,10 +2646,10 @@
         <v>258</v>
       </c>
       <c r="C119" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="D119" t="s">
-        <v>279</v>
+        <v>245</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -2660,10 +2660,10 @@
         <v>259</v>
       </c>
       <c r="C120" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D120" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
     </row>
     <row r="121" spans="1:4">
@@ -2674,7 +2674,7 @@
         <v>260</v>
       </c>
       <c r="C121" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D121" t="s">
         <v>245</v>
@@ -2688,7 +2688,7 @@
         <v>261</v>
       </c>
       <c r="C122" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
     </row>
     <row r="123" spans="1:4">
@@ -2729,7 +2729,7 @@
         <v>249</v>
       </c>
       <c r="C126" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D126" t="s">
         <v>259</v>
@@ -2743,10 +2743,10 @@
         <v>250</v>
       </c>
       <c r="C127" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D127" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -2757,7 +2757,7 @@
         <v>251</v>
       </c>
       <c r="C128" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D128" t="s">
         <v>246</v>
@@ -2771,7 +2771,7 @@
         <v>252</v>
       </c>
       <c r="C129" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -2782,7 +2782,7 @@
         <v>253</v>
       </c>
       <c r="C130" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
     </row>
     <row r="131" spans="1:4">
@@ -2793,7 +2793,7 @@
         <v>253</v>
       </c>
       <c r="C131" t="s">
-        <v>278</v>
+        <v>245</v>
       </c>
     </row>
     <row r="132" spans="1:4">
@@ -2804,7 +2804,7 @@
         <v>253</v>
       </c>
       <c r="C132" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="D132" t="s">
         <v>245</v>
@@ -2826,7 +2826,7 @@
         <v>252</v>
       </c>
       <c r="D134" t="s">
-        <v>281</v>
+        <v>261</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -2837,7 +2837,7 @@
         <v>251</v>
       </c>
       <c r="C135" t="s">
-        <v>251</v>
+        <v>272</v>
       </c>
       <c r="D135" t="s">
         <v>245</v>
@@ -2862,10 +2862,10 @@
         <v>250</v>
       </c>
       <c r="C137" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D137" t="s">
-        <v>281</v>
+        <v>261</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -2876,7 +2876,7 @@
         <v>250</v>
       </c>
       <c r="C138" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D138" t="s">
         <v>259</v>
@@ -2893,7 +2893,7 @@
         <v>276</v>
       </c>
       <c r="D139" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
     </row>
     <row r="140" spans="1:4">
@@ -2904,7 +2904,7 @@
         <v>259</v>
       </c>
       <c r="C140" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D140" t="s">
         <v>245</v>
@@ -2918,7 +2918,7 @@
         <v>260</v>
       </c>
       <c r="C141" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D141" t="s">
         <v>248</v>
@@ -2932,10 +2932,10 @@
         <v>261</v>
       </c>
       <c r="C142" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D142" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="143" spans="1:4">
@@ -2946,7 +2946,7 @@
         <v>262</v>
       </c>
       <c r="C143" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="D143" t="s">
         <v>246</v>
@@ -2960,10 +2960,10 @@
         <v>263</v>
       </c>
       <c r="C144" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D144" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="145" spans="1:4">
@@ -2974,7 +2974,7 @@
         <v>264</v>
       </c>
       <c r="C145" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D145" t="s">
         <v>245</v>
@@ -2988,10 +2988,10 @@
         <v>249</v>
       </c>
       <c r="C146" t="s">
-        <v>267</v>
+        <v>252</v>
       </c>
       <c r="D146" t="s">
-        <v>279</v>
+        <v>261</v>
       </c>
     </row>
     <row r="147" spans="1:4">
@@ -3013,7 +3013,7 @@
         <v>247</v>
       </c>
       <c r="D148" t="s">
-        <v>281</v>
+        <v>261</v>
       </c>
     </row>
     <row r="149" spans="1:4">
@@ -3024,10 +3024,10 @@
         <v>264</v>
       </c>
       <c r="C149" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D149" t="s">
-        <v>281</v>
+        <v>260</v>
       </c>
     </row>
     <row r="150" spans="1:4">
@@ -3038,10 +3038,10 @@
         <v>263</v>
       </c>
       <c r="C150" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D150" t="s">
-        <v>279</v>
+        <v>261</v>
       </c>
     </row>
     <row r="151" spans="1:4">
@@ -3052,7 +3052,7 @@
         <v>263</v>
       </c>
       <c r="C151" t="s">
-        <v>277</v>
+        <v>250</v>
       </c>
       <c r="D151" t="s">
         <v>246</v>
@@ -3066,10 +3066,10 @@
         <v>262</v>
       </c>
       <c r="C152" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D152" t="s">
-        <v>248</v>
+        <v>280</v>
       </c>
     </row>
     <row r="153" spans="1:4">
@@ -3080,7 +3080,7 @@
         <v>262</v>
       </c>
       <c r="C153" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="154" spans="1:4">
@@ -3126,7 +3126,7 @@
         <v>259</v>
       </c>
       <c r="C158" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="159" spans="1:4">
@@ -3137,10 +3137,10 @@
         <v>258</v>
       </c>
       <c r="C159" t="s">
-        <v>272</v>
+        <v>250</v>
       </c>
       <c r="D159" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="160" spans="1:4">
@@ -3151,10 +3151,10 @@
         <v>259</v>
       </c>
       <c r="C160" t="s">
-        <v>274</v>
+        <v>250</v>
       </c>
       <c r="D160" t="s">
-        <v>261</v>
+        <v>245</v>
       </c>
     </row>
     <row r="161" spans="1:4">
@@ -3165,7 +3165,7 @@
         <v>258</v>
       </c>
       <c r="C161" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="162" spans="1:4">
@@ -3176,7 +3176,7 @@
         <v>265</v>
       </c>
       <c r="C162" t="s">
-        <v>268</v>
+        <v>252</v>
       </c>
       <c r="D162" t="s">
         <v>246</v>
@@ -3190,10 +3190,10 @@
         <v>265</v>
       </c>
       <c r="C163" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D163" t="s">
-        <v>281</v>
+        <v>261</v>
       </c>
     </row>
     <row r="164" spans="1:4">
@@ -3204,7 +3204,7 @@
         <v>265</v>
       </c>
       <c r="C164" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="165" spans="1:4">
@@ -3215,7 +3215,7 @@
         <v>265</v>
       </c>
       <c r="C165" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="D165" t="s">
         <v>246</v>
@@ -3242,7 +3242,7 @@
         <v>170</v>
       </c>
       <c r="C168" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="169" spans="1:4">
@@ -3250,7 +3250,7 @@
         <v>171</v>
       </c>
       <c r="C169" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="170" spans="1:4">
@@ -3258,10 +3258,10 @@
         <v>172</v>
       </c>
       <c r="C170" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="D170" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="171" spans="1:4">
@@ -3285,7 +3285,7 @@
         <v>175</v>
       </c>
       <c r="C173" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
     </row>
     <row r="174" spans="1:4">
@@ -3301,7 +3301,7 @@
         <v>177</v>
       </c>
       <c r="C175" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="176" spans="1:4">
@@ -3317,7 +3317,7 @@
         <v>179</v>
       </c>
       <c r="C177" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D177" t="s">
         <v>261</v>
@@ -3336,10 +3336,10 @@
         <v>181</v>
       </c>
       <c r="C179" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="D179" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="180" spans="1:4">
@@ -3355,7 +3355,7 @@
         <v>183</v>
       </c>
       <c r="C181" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D181" t="s">
         <v>259</v>
@@ -3366,7 +3366,7 @@
         <v>184</v>
       </c>
       <c r="C182" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D182" t="s">
         <v>260</v>
@@ -3377,7 +3377,7 @@
         <v>185</v>
       </c>
       <c r="C183" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="184" spans="1:4">
@@ -3385,7 +3385,7 @@
         <v>186</v>
       </c>
       <c r="C184" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="185" spans="1:4">
@@ -3393,7 +3393,7 @@
         <v>187</v>
       </c>
       <c r="C185" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="186" spans="1:4">
@@ -3401,7 +3401,7 @@
         <v>188</v>
       </c>
       <c r="C186" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="187" spans="1:4">
@@ -3417,7 +3417,7 @@
         <v>190</v>
       </c>
       <c r="C188" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D188" t="s">
         <v>259</v>
@@ -3428,7 +3428,7 @@
         <v>191</v>
       </c>
       <c r="C189" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="190" spans="1:4">
@@ -3436,7 +3436,7 @@
         <v>192</v>
       </c>
       <c r="C190" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row r="191" spans="1:4">
@@ -3463,7 +3463,7 @@
         <v>195</v>
       </c>
       <c r="C193" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D193" t="s">
         <v>248</v>
@@ -3474,7 +3474,7 @@
         <v>196</v>
       </c>
       <c r="C194" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="195" spans="1:4">
@@ -3482,7 +3482,7 @@
         <v>197</v>
       </c>
       <c r="C195" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D195" t="s">
         <v>260</v>
@@ -3493,10 +3493,10 @@
         <v>198</v>
       </c>
       <c r="C196" t="s">
-        <v>252</v>
+        <v>268</v>
       </c>
       <c r="D196" t="s">
-        <v>248</v>
+        <v>281</v>
       </c>
     </row>
     <row r="197" spans="1:4">
@@ -3504,7 +3504,7 @@
         <v>199</v>
       </c>
       <c r="C197" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="D197" t="s">
         <v>261</v>
@@ -3515,7 +3515,7 @@
         <v>200</v>
       </c>
       <c r="C198" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
     </row>
     <row r="199" spans="1:4">
@@ -3523,7 +3523,7 @@
         <v>201</v>
       </c>
       <c r="C199" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D199" t="s">
         <v>281</v>
@@ -3534,7 +3534,7 @@
         <v>202</v>
       </c>
       <c r="C200" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="201" spans="1:4">
@@ -3542,7 +3542,7 @@
         <v>203</v>
       </c>
       <c r="C201" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="D201" t="s">
         <v>245</v>
@@ -3553,7 +3553,7 @@
         <v>204</v>
       </c>
       <c r="C202" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="203" spans="1:4">
@@ -3561,7 +3561,7 @@
         <v>205</v>
       </c>
       <c r="C203" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="204" spans="1:4">
@@ -3569,7 +3569,7 @@
         <v>206</v>
       </c>
       <c r="C204" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="D204" t="s">
         <v>261</v>
@@ -3580,7 +3580,7 @@
         <v>207</v>
       </c>
       <c r="C205" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
     </row>
     <row r="206" spans="1:4">
@@ -3588,7 +3588,7 @@
         <v>208</v>
       </c>
       <c r="C206" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="207" spans="1:4">
@@ -3596,7 +3596,7 @@
         <v>209</v>
       </c>
       <c r="C207" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
     </row>
     <row r="208" spans="1:4">
@@ -3604,7 +3604,7 @@
         <v>210</v>
       </c>
       <c r="D208" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="209" spans="1:4">
@@ -3612,7 +3612,7 @@
         <v>211</v>
       </c>
       <c r="D209" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="210" spans="1:4">
@@ -3620,7 +3620,7 @@
         <v>212</v>
       </c>
       <c r="D210" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="211" spans="1:4">
@@ -3628,7 +3628,7 @@
         <v>213</v>
       </c>
       <c r="D211" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="212" spans="1:4">
@@ -3636,7 +3636,7 @@
         <v>214</v>
       </c>
       <c r="D212" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="213" spans="1:4">
@@ -3652,7 +3652,7 @@
         <v>216</v>
       </c>
       <c r="D214" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="215" spans="1:4">
@@ -3660,7 +3660,7 @@
         <v>217</v>
       </c>
       <c r="D215" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="216" spans="1:4">
@@ -3668,7 +3668,7 @@
         <v>218</v>
       </c>
       <c r="D216" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="217" spans="1:4">
@@ -3676,7 +3676,7 @@
         <v>219</v>
       </c>
       <c r="D217" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="218" spans="1:4">
@@ -3684,7 +3684,7 @@
         <v>220</v>
       </c>
       <c r="D218" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="219" spans="1:4">
@@ -3692,7 +3692,7 @@
         <v>221</v>
       </c>
       <c r="D219" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="220" spans="1:4">
@@ -3700,7 +3700,7 @@
         <v>222</v>
       </c>
       <c r="D220" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="221" spans="1:4">
@@ -3708,7 +3708,7 @@
         <v>223</v>
       </c>
       <c r="D221" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="222" spans="1:4">
@@ -3724,7 +3724,7 @@
         <v>225</v>
       </c>
       <c r="D223" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="224" spans="1:4">
@@ -3732,7 +3732,7 @@
         <v>226</v>
       </c>
       <c r="D224" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="225" spans="1:4">
@@ -3740,7 +3740,7 @@
         <v>227</v>
       </c>
       <c r="D225" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="226" spans="1:4">
@@ -3764,7 +3764,7 @@
         <v>230</v>
       </c>
       <c r="D228" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="229" spans="1:4">
@@ -3860,7 +3860,7 @@
         <v>242</v>
       </c>
       <c r="D240" t="s">
-        <v>281</v>
+        <v>261</v>
       </c>
     </row>
     <row r="241" spans="1:4">
@@ -3876,7 +3876,7 @@
         <v>244</v>
       </c>
       <c r="D242" t="s">
-        <v>281</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactoriza con asigna_subgrupo_estudiante_semanas() renombre variables
</commit_message>
<xml_diff>
--- a/lista_subgrupos.xlsx
+++ b/lista_subgrupos.xlsx
@@ -757,109 +757,109 @@
     <t>MI11-B</t>
   </si>
   <si>
+    <t>MI11-C</t>
+  </si>
+  <si>
+    <t>MI09-D</t>
+  </si>
+  <si>
+    <t>MI09-C</t>
+  </si>
+  <si>
+    <t>MI09-B</t>
+  </si>
+  <si>
+    <t>MI09-A</t>
+  </si>
+  <si>
+    <t>VI11-D</t>
+  </si>
+  <si>
+    <t>VI11-C</t>
+  </si>
+  <si>
+    <t>VI11-B</t>
+  </si>
+  <si>
+    <t>VI11-A</t>
+  </si>
+  <si>
+    <t>JU11-D</t>
+  </si>
+  <si>
+    <t>JU11-C</t>
+  </si>
+  <si>
+    <t>JU11-B</t>
+  </si>
+  <si>
+    <t>JU11-A</t>
+  </si>
+  <si>
+    <t>JU09-D</t>
+  </si>
+  <si>
+    <t>JU09-C</t>
+  </si>
+  <si>
+    <t>JU09-B</t>
+  </si>
+  <si>
+    <t>JU09-A</t>
+  </si>
+  <si>
     <t>MI11-D</t>
   </si>
   <si>
-    <t>MI11-C</t>
-  </si>
-  <si>
-    <t>VI11-A</t>
-  </si>
-  <si>
-    <t>JU11-D</t>
-  </si>
-  <si>
-    <t>JU11-C</t>
-  </si>
-  <si>
-    <t>JU11-B</t>
-  </si>
-  <si>
-    <t>JU11-A</t>
-  </si>
-  <si>
-    <t>JU09-D</t>
-  </si>
-  <si>
-    <t>JU09-C</t>
-  </si>
-  <si>
-    <t>JU09-B</t>
-  </si>
-  <si>
-    <t>JU09-A</t>
-  </si>
-  <si>
-    <t>MI09-D</t>
-  </si>
-  <si>
-    <t>MI09-C</t>
-  </si>
-  <si>
-    <t>MI09-B</t>
-  </si>
-  <si>
-    <t>MI09-A</t>
-  </si>
-  <si>
-    <t>VI11-D</t>
-  </si>
-  <si>
-    <t>VI11-C</t>
-  </si>
-  <si>
-    <t>VI11-B</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
+    <t>MI11-E</t>
+  </si>
+  <si>
+    <t>MI11-G</t>
+  </si>
+  <si>
+    <t>JU11-F</t>
+  </si>
+  <si>
+    <t>JU11-E</t>
+  </si>
+  <si>
+    <t>VI09-C</t>
+  </si>
+  <si>
+    <t>VI09-E</t>
+  </si>
+  <si>
     <t>MI11-F</t>
   </si>
   <si>
-    <t>MI11-G</t>
-  </si>
-  <si>
-    <t>MI11-E</t>
+    <t>VI09-G</t>
+  </si>
+  <si>
+    <t>VI09-F</t>
+  </si>
+  <si>
+    <t>VI09-D</t>
   </si>
   <si>
     <t>VI09-B</t>
   </si>
   <si>
-    <t>VI09-G</t>
+    <t>JU11-G</t>
   </si>
   <si>
     <t>VI09-A</t>
   </si>
   <si>
-    <t>VI09-F</t>
-  </si>
-  <si>
-    <t>JU11-F</t>
-  </si>
-  <si>
-    <t>VI09-C</t>
-  </si>
-  <si>
-    <t>JU11-G</t>
-  </si>
-  <si>
-    <t>VI09-E</t>
-  </si>
-  <si>
-    <t>VI09-D</t>
-  </si>
-  <si>
-    <t>JU11-E</t>
-  </si>
-  <si>
     <t>MA11-A</t>
   </si>
   <si>
+    <t>MA11-C</t>
+  </si>
+  <si>
     <t>MA11-B</t>
-  </si>
-  <si>
-    <t>MA11-C</t>
   </si>
 </sst>
 </file>
@@ -1245,7 +1245,7 @@
         <v>245</v>
       </c>
       <c r="C2" t="s">
-        <v>266</v>
+        <v>245</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1264,10 +1264,10 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C4" t="s">
-        <v>266</v>
+        <v>246</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1297,7 +1297,7 @@
         <v>245</v>
       </c>
       <c r="C7" t="s">
-        <v>247</v>
+        <v>266</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1308,7 +1308,7 @@
         <v>245</v>
       </c>
       <c r="C8" t="s">
-        <v>266</v>
+        <v>245</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1319,7 +1319,7 @@
         <v>245</v>
       </c>
       <c r="C9" t="s">
-        <v>267</v>
+        <v>245</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1327,7 +1327,7 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1338,7 +1338,7 @@
         <v>246</v>
       </c>
       <c r="C11" t="s">
-        <v>267</v>
+        <v>246</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1349,7 +1349,7 @@
         <v>246</v>
       </c>
       <c r="C12" t="s">
-        <v>267</v>
+        <v>246</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1357,10 +1357,10 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C13" t="s">
-        <v>268</v>
+        <v>245</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1371,7 +1371,7 @@
         <v>246</v>
       </c>
       <c r="C14" t="s">
-        <v>266</v>
+        <v>246</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1379,10 +1379,10 @@
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C15" t="s">
-        <v>267</v>
+        <v>246</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1390,10 +1390,10 @@
         <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C16" t="s">
-        <v>266</v>
+        <v>246</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1404,7 +1404,7 @@
         <v>246</v>
       </c>
       <c r="C17" t="s">
-        <v>266</v>
+        <v>246</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1415,7 +1415,7 @@
         <v>246</v>
       </c>
       <c r="C18" t="s">
-        <v>266</v>
+        <v>246</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1423,10 +1423,10 @@
         <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C19" t="s">
-        <v>267</v>
+        <v>245</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1434,10 +1434,10 @@
         <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C20" t="s">
-        <v>267</v>
+        <v>245</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1445,10 +1445,10 @@
         <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C21" t="s">
-        <v>267</v>
+        <v>247</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1456,7 +1456,7 @@
         <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D22" t="s">
         <v>279</v>
@@ -1467,10 +1467,10 @@
         <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C23" t="s">
-        <v>266</v>
+        <v>245</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1478,10 +1478,10 @@
         <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C24" t="s">
-        <v>267</v>
+        <v>245</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1489,7 +1489,7 @@
         <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1497,13 +1497,13 @@
         <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C26" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D26" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1511,13 +1511,13 @@
         <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C27" t="s">
-        <v>247</v>
+        <v>267</v>
       </c>
       <c r="D27" t="s">
-        <v>261</v>
+        <v>280</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1525,10 +1525,10 @@
         <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C28" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="D28" t="s">
         <v>280</v>
@@ -1539,7 +1539,7 @@
         <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1547,10 +1547,10 @@
         <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D30" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1558,13 +1558,13 @@
         <v>33</v>
       </c>
       <c r="B31" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C31" t="s">
-        <v>253</v>
+        <v>268</v>
       </c>
       <c r="D31" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1572,13 +1572,13 @@
         <v>34</v>
       </c>
       <c r="B32" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C32" t="s">
-        <v>270</v>
+        <v>247</v>
       </c>
       <c r="D32" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1586,13 +1586,13 @@
         <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C33" t="s">
-        <v>253</v>
+        <v>269</v>
       </c>
       <c r="D33" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1600,13 +1600,13 @@
         <v>36</v>
       </c>
       <c r="B34" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C34" t="s">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="D34" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1614,13 +1614,13 @@
         <v>37</v>
       </c>
       <c r="B35" t="s">
-        <v>247</v>
+        <v>257</v>
       </c>
       <c r="C35" t="s">
         <v>271</v>
       </c>
       <c r="D35" t="s">
-        <v>280</v>
+        <v>247</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1628,13 +1628,13 @@
         <v>38</v>
       </c>
       <c r="B36" t="s">
-        <v>248</v>
+        <v>258</v>
       </c>
       <c r="C36" t="s">
         <v>272</v>
       </c>
       <c r="D36" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1642,13 +1642,13 @@
         <v>39</v>
       </c>
       <c r="B37" t="s">
-        <v>247</v>
+        <v>259</v>
       </c>
       <c r="C37" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D37" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1656,7 +1656,7 @@
         <v>40</v>
       </c>
       <c r="B38" t="s">
-        <v>247</v>
+        <v>260</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1664,10 +1664,10 @@
         <v>41</v>
       </c>
       <c r="B39" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="C39" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="D39" t="s">
         <v>245</v>
@@ -1678,10 +1678,10 @@
         <v>42</v>
       </c>
       <c r="B40" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="D40" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1689,7 +1689,7 @@
         <v>43</v>
       </c>
       <c r="B41" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1697,10 +1697,10 @@
         <v>44</v>
       </c>
       <c r="B42" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="C42" t="s">
-        <v>245</v>
+        <v>264</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1708,13 +1708,13 @@
         <v>45</v>
       </c>
       <c r="B43" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="C43" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="D43" t="s">
-        <v>246</v>
+        <v>279</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1722,7 +1722,7 @@
         <v>46</v>
       </c>
       <c r="B44" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1730,13 +1730,13 @@
         <v>47</v>
       </c>
       <c r="B45" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="C45" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D45" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1744,10 +1744,10 @@
         <v>48</v>
       </c>
       <c r="B46" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="C46" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1755,10 +1755,10 @@
         <v>49</v>
       </c>
       <c r="B47" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="C47" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1766,10 +1766,10 @@
         <v>50</v>
       </c>
       <c r="B48" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="C48" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1777,13 +1777,13 @@
         <v>51</v>
       </c>
       <c r="B49" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="C49" t="s">
-        <v>248</v>
+        <v>273</v>
       </c>
       <c r="D49" t="s">
-        <v>280</v>
+        <v>247</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1791,10 +1791,10 @@
         <v>52</v>
       </c>
       <c r="B50" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="D50" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1802,10 +1802,10 @@
         <v>53</v>
       </c>
       <c r="B51" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C51" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1813,10 +1813,10 @@
         <v>54</v>
       </c>
       <c r="B52" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="C52" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1824,13 +1824,13 @@
         <v>55</v>
       </c>
       <c r="B53" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="C53" t="s">
-        <v>270</v>
+        <v>247</v>
       </c>
       <c r="D53" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1838,10 +1838,10 @@
         <v>56</v>
       </c>
       <c r="B54" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="C54" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1849,10 +1849,10 @@
         <v>57</v>
       </c>
       <c r="B55" t="s">
+        <v>261</v>
+      </c>
+      <c r="D55" t="s">
         <v>247</v>
-      </c>
-      <c r="D55" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -1860,10 +1860,10 @@
         <v>58</v>
       </c>
       <c r="B56" t="s">
-        <v>247</v>
+        <v>262</v>
       </c>
       <c r="D56" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1871,13 +1871,13 @@
         <v>59</v>
       </c>
       <c r="B57" t="s">
-        <v>247</v>
+        <v>263</v>
       </c>
       <c r="C57" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="D57" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -1885,13 +1885,13 @@
         <v>60</v>
       </c>
       <c r="B58" t="s">
+        <v>264</v>
+      </c>
+      <c r="C58" t="s">
+        <v>270</v>
+      </c>
+      <c r="D58" t="s">
         <v>247</v>
-      </c>
-      <c r="C58" t="s">
-        <v>273</v>
-      </c>
-      <c r="D58" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -1899,10 +1899,10 @@
         <v>61</v>
       </c>
       <c r="B59" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="C59" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -1910,10 +1910,10 @@
         <v>62</v>
       </c>
       <c r="B60" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="C60" t="s">
-        <v>248</v>
+        <v>257</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -1921,13 +1921,13 @@
         <v>63</v>
       </c>
       <c r="B61" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="C61" t="s">
-        <v>247</v>
+        <v>272</v>
       </c>
       <c r="D61" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -1935,10 +1935,10 @@
         <v>64</v>
       </c>
       <c r="B62" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="D62" t="s">
-        <v>245</v>
+        <v>280</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -1946,10 +1946,10 @@
         <v>65</v>
       </c>
       <c r="B63" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="C63" t="s">
-        <v>246</v>
+        <v>259</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -1957,13 +1957,13 @@
         <v>66</v>
       </c>
       <c r="B64" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="C64" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="D64" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -1971,10 +1971,10 @@
         <v>67</v>
       </c>
       <c r="B65" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="C65" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D65" t="s">
         <v>245</v>
@@ -1985,10 +1985,10 @@
         <v>68</v>
       </c>
       <c r="B66" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="C66" t="s">
-        <v>246</v>
+        <v>266</v>
       </c>
       <c r="D66" t="s">
         <v>280</v>
@@ -1999,13 +1999,13 @@
         <v>69</v>
       </c>
       <c r="B67" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="C67" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="D67" t="s">
-        <v>248</v>
+        <v>279</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -2013,13 +2013,13 @@
         <v>70</v>
       </c>
       <c r="B68" t="s">
-        <v>251</v>
+        <v>258</v>
       </c>
       <c r="C68" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D68" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -2027,10 +2027,10 @@
         <v>71</v>
       </c>
       <c r="B69" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="C69" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -2038,13 +2038,13 @@
         <v>72</v>
       </c>
       <c r="B70" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="C70" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="D70" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -2052,13 +2052,13 @@
         <v>73</v>
       </c>
       <c r="B71" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="C71" t="s">
-        <v>253</v>
+        <v>277</v>
       </c>
       <c r="D71" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -2066,7 +2066,7 @@
         <v>74</v>
       </c>
       <c r="B72" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -2074,7 +2074,7 @@
         <v>75</v>
       </c>
       <c r="B73" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -2082,10 +2082,10 @@
         <v>76</v>
       </c>
       <c r="B74" t="s">
+        <v>264</v>
+      </c>
+      <c r="C74" t="s">
         <v>257</v>
-      </c>
-      <c r="C74" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -2093,10 +2093,10 @@
         <v>77</v>
       </c>
       <c r="B75" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
       <c r="C75" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
       <c r="D75" t="s">
         <v>279</v>
@@ -2107,7 +2107,7 @@
         <v>78</v>
       </c>
       <c r="B76" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -2115,7 +2115,7 @@
         <v>79</v>
       </c>
       <c r="B77" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -2123,7 +2123,7 @@
         <v>80</v>
       </c>
       <c r="B78" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -2131,13 +2131,13 @@
         <v>81</v>
       </c>
       <c r="B79" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C79" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D79" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -2145,13 +2145,13 @@
         <v>82</v>
       </c>
       <c r="B80" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C80" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="D80" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -2159,13 +2159,13 @@
         <v>83</v>
       </c>
       <c r="B81" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C81" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="D81" t="s">
-        <v>281</v>
+        <v>250</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -2173,10 +2173,10 @@
         <v>84</v>
       </c>
       <c r="B82" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C82" t="s">
-        <v>250</v>
+        <v>278</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -2184,13 +2184,13 @@
         <v>85</v>
       </c>
       <c r="B83" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C83" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D83" t="s">
-        <v>281</v>
+        <v>250</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -2198,10 +2198,10 @@
         <v>86</v>
       </c>
       <c r="B84" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C84" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="D84" t="s">
         <v>281</v>
@@ -2212,13 +2212,13 @@
         <v>87</v>
       </c>
       <c r="B85" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C85" t="s">
-        <v>248</v>
+        <v>278</v>
       </c>
       <c r="D85" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -2226,7 +2226,7 @@
         <v>88</v>
       </c>
       <c r="B86" t="s">
-        <v>249</v>
+        <v>261</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -2234,13 +2234,13 @@
         <v>89</v>
       </c>
       <c r="B87" t="s">
-        <v>250</v>
+        <v>262</v>
       </c>
       <c r="C87" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="D87" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -2248,13 +2248,13 @@
         <v>90</v>
       </c>
       <c r="B88" t="s">
-        <v>251</v>
+        <v>263</v>
       </c>
       <c r="C88" t="s">
-        <v>246</v>
+        <v>264</v>
       </c>
       <c r="D88" t="s">
-        <v>260</v>
+        <v>281</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -2262,10 +2262,10 @@
         <v>91</v>
       </c>
       <c r="B89" t="s">
-        <v>252</v>
+        <v>263</v>
       </c>
       <c r="C89" t="s">
-        <v>246</v>
+        <v>268</v>
       </c>
       <c r="D89" t="s">
         <v>281</v>
@@ -2276,13 +2276,13 @@
         <v>92</v>
       </c>
       <c r="B90" t="s">
-        <v>253</v>
+        <v>263</v>
       </c>
       <c r="C90" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="D90" t="s">
-        <v>246</v>
+        <v>280</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -2290,13 +2290,13 @@
         <v>93</v>
       </c>
       <c r="B91" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="C91" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D91" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -2304,10 +2304,10 @@
         <v>94</v>
       </c>
       <c r="B92" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C92" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -2315,13 +2315,13 @@
         <v>95</v>
       </c>
       <c r="B93" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C93" t="s">
-        <v>275</v>
+        <v>257</v>
       </c>
       <c r="D93" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -2329,13 +2329,13 @@
         <v>96</v>
       </c>
       <c r="B94" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C94" t="s">
-        <v>252</v>
+        <v>266</v>
       </c>
       <c r="D94" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -2343,13 +2343,13 @@
         <v>97</v>
       </c>
       <c r="B95" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C95" t="s">
         <v>277</v>
       </c>
       <c r="D95" t="s">
-        <v>281</v>
+        <v>250</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -2357,10 +2357,10 @@
         <v>98</v>
       </c>
       <c r="B96" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C96" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -2371,7 +2371,7 @@
         <v>256</v>
       </c>
       <c r="D97" t="s">
-        <v>261</v>
+        <v>245</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -2379,10 +2379,10 @@
         <v>100</v>
       </c>
       <c r="B98" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C98" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -2393,10 +2393,10 @@
         <v>258</v>
       </c>
       <c r="C99" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D99" t="s">
-        <v>248</v>
+        <v>281</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -2407,10 +2407,10 @@
         <v>259</v>
       </c>
       <c r="C100" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="D100" t="s">
-        <v>280</v>
+        <v>245</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -2429,10 +2429,10 @@
         <v>261</v>
       </c>
       <c r="C102" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="D102" t="s">
-        <v>281</v>
+        <v>245</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -2443,7 +2443,7 @@
         <v>262</v>
       </c>
       <c r="D103" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -2454,10 +2454,10 @@
         <v>263</v>
       </c>
       <c r="C104" t="s">
-        <v>247</v>
+        <v>276</v>
       </c>
       <c r="D104" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -2465,13 +2465,13 @@
         <v>107</v>
       </c>
       <c r="B105" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C105" t="s">
-        <v>245</v>
+        <v>275</v>
       </c>
       <c r="D105" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -2479,13 +2479,13 @@
         <v>108</v>
       </c>
       <c r="B106" t="s">
-        <v>249</v>
+        <v>262</v>
       </c>
       <c r="C106" t="s">
-        <v>250</v>
+        <v>278</v>
       </c>
       <c r="D106" t="s">
-        <v>260</v>
+        <v>280</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -2493,13 +2493,13 @@
         <v>109</v>
       </c>
       <c r="B107" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="C107" t="s">
-        <v>245</v>
+        <v>268</v>
       </c>
       <c r="D107" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -2507,13 +2507,13 @@
         <v>110</v>
       </c>
       <c r="B108" t="s">
+        <v>254</v>
+      </c>
+      <c r="C108" t="s">
+        <v>256</v>
+      </c>
+      <c r="D108" t="s">
         <v>251</v>
-      </c>
-      <c r="C108" t="s">
-        <v>269</v>
-      </c>
-      <c r="D108" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -2521,10 +2521,10 @@
         <v>111</v>
       </c>
       <c r="B109" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="D109" t="s">
-        <v>260</v>
+        <v>281</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -2532,13 +2532,13 @@
         <v>112</v>
       </c>
       <c r="B110" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="C110" t="s">
-        <v>274</v>
+        <v>258</v>
       </c>
       <c r="D110" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -2546,7 +2546,7 @@
         <v>113</v>
       </c>
       <c r="B111" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -2554,10 +2554,10 @@
         <v>114</v>
       </c>
       <c r="B112" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="C112" t="s">
-        <v>248</v>
+        <v>264</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -2565,7 +2565,7 @@
         <v>115</v>
       </c>
       <c r="B113" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -2573,13 +2573,13 @@
         <v>116</v>
       </c>
       <c r="B114" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="C114" t="s">
-        <v>248</v>
+        <v>268</v>
       </c>
       <c r="D114" t="s">
-        <v>280</v>
+        <v>245</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -2587,13 +2587,13 @@
         <v>117</v>
       </c>
       <c r="B115" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="C115" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="D115" t="s">
-        <v>245</v>
+        <v>280</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -2601,13 +2601,13 @@
         <v>118</v>
       </c>
       <c r="B116" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="C116" t="s">
+        <v>272</v>
+      </c>
+      <c r="D116" t="s">
         <v>251</v>
-      </c>
-      <c r="D116" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -2615,13 +2615,13 @@
         <v>119</v>
       </c>
       <c r="B117" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="C117" t="s">
-        <v>251</v>
+        <v>277</v>
       </c>
       <c r="D117" t="s">
-        <v>281</v>
+        <v>250</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -2629,13 +2629,13 @@
         <v>120</v>
       </c>
       <c r="B118" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="C118" t="s">
-        <v>246</v>
+        <v>277</v>
       </c>
       <c r="D118" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
     </row>
     <row r="119" spans="1:4">
@@ -2643,13 +2643,13 @@
         <v>121</v>
       </c>
       <c r="B119" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="C119" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="D119" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -2657,10 +2657,10 @@
         <v>122</v>
       </c>
       <c r="B120" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="C120" t="s">
-        <v>250</v>
+        <v>269</v>
       </c>
       <c r="D120" t="s">
         <v>245</v>
@@ -2671,13 +2671,13 @@
         <v>123</v>
       </c>
       <c r="B121" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="C121" t="s">
-        <v>277</v>
+        <v>258</v>
       </c>
       <c r="D121" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -2685,10 +2685,10 @@
         <v>124</v>
       </c>
       <c r="B122" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="C122" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
     </row>
     <row r="123" spans="1:4">
@@ -2696,7 +2696,7 @@
         <v>125</v>
       </c>
       <c r="B123" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
     </row>
     <row r="124" spans="1:4">
@@ -2704,13 +2704,13 @@
         <v>126</v>
       </c>
       <c r="B124" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="C124" t="s">
-        <v>276</v>
+        <v>257</v>
       </c>
       <c r="D124" t="s">
-        <v>248</v>
+        <v>280</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -2718,7 +2718,7 @@
         <v>127</v>
       </c>
       <c r="B125" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
     </row>
     <row r="126" spans="1:4">
@@ -2726,13 +2726,13 @@
         <v>128</v>
       </c>
       <c r="B126" t="s">
-        <v>249</v>
+        <v>259</v>
       </c>
       <c r="C126" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="D126" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
     </row>
     <row r="127" spans="1:4">
@@ -2740,13 +2740,13 @@
         <v>129</v>
       </c>
       <c r="B127" t="s">
-        <v>250</v>
+        <v>260</v>
       </c>
       <c r="C127" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D127" t="s">
-        <v>281</v>
+        <v>249</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -2754,13 +2754,13 @@
         <v>130</v>
       </c>
       <c r="B128" t="s">
-        <v>251</v>
+        <v>260</v>
       </c>
       <c r="C128" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="D128" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
     </row>
     <row r="129" spans="1:4">
@@ -2768,10 +2768,10 @@
         <v>131</v>
       </c>
       <c r="B129" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="C129" t="s">
-        <v>277</v>
+        <v>259</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -2779,10 +2779,10 @@
         <v>132</v>
       </c>
       <c r="B130" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="C130" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="131" spans="1:4">
@@ -2790,10 +2790,10 @@
         <v>133</v>
       </c>
       <c r="B131" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C131" t="s">
-        <v>245</v>
+        <v>270</v>
       </c>
     </row>
     <row r="132" spans="1:4">
@@ -2801,10 +2801,10 @@
         <v>134</v>
       </c>
       <c r="B132" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C132" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D132" t="s">
         <v>245</v>
@@ -2815,7 +2815,7 @@
         <v>135</v>
       </c>
       <c r="B133" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -2826,7 +2826,7 @@
         <v>252</v>
       </c>
       <c r="D134" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -2834,13 +2834,13 @@
         <v>137</v>
       </c>
       <c r="B135" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C135" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="D135" t="s">
-        <v>245</v>
+        <v>281</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -2848,10 +2848,10 @@
         <v>138</v>
       </c>
       <c r="B136" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="D136" t="s">
-        <v>261</v>
+        <v>280</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -2859,13 +2859,13 @@
         <v>139</v>
       </c>
       <c r="B137" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="C137" t="s">
-        <v>272</v>
+        <v>256</v>
       </c>
       <c r="D137" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -2873,13 +2873,13 @@
         <v>140</v>
       </c>
       <c r="B138" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="C138" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="D138" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
     </row>
     <row r="139" spans="1:4">
@@ -2887,13 +2887,13 @@
         <v>141</v>
       </c>
       <c r="B139" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C139" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="D139" t="s">
-        <v>245</v>
+        <v>281</v>
       </c>
     </row>
     <row r="140" spans="1:4">
@@ -2901,13 +2901,13 @@
         <v>142</v>
       </c>
       <c r="B140" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C140" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="D140" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
     </row>
     <row r="141" spans="1:4">
@@ -2915,13 +2915,13 @@
         <v>143</v>
       </c>
       <c r="B141" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="C141" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="D141" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="142" spans="1:4">
@@ -2929,13 +2929,13 @@
         <v>144</v>
       </c>
       <c r="B142" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="C142" t="s">
         <v>270</v>
       </c>
       <c r="D142" t="s">
-        <v>281</v>
+        <v>249</v>
       </c>
     </row>
     <row r="143" spans="1:4">
@@ -2943,13 +2943,13 @@
         <v>145</v>
       </c>
       <c r="B143" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="C143" t="s">
-        <v>274</v>
+        <v>256</v>
       </c>
       <c r="D143" t="s">
-        <v>246</v>
+        <v>281</v>
       </c>
     </row>
     <row r="144" spans="1:4">
@@ -2957,13 +2957,13 @@
         <v>146</v>
       </c>
       <c r="B144" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
       <c r="C144" t="s">
-        <v>252</v>
+        <v>266</v>
       </c>
       <c r="D144" t="s">
-        <v>280</v>
+        <v>246</v>
       </c>
     </row>
     <row r="145" spans="1:4">
@@ -2971,13 +2971,13 @@
         <v>147</v>
       </c>
       <c r="B145" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="C145" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D145" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
     </row>
     <row r="146" spans="1:4">
@@ -2985,13 +2985,13 @@
         <v>148</v>
       </c>
       <c r="B146" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C146" t="s">
-        <v>252</v>
+        <v>272</v>
       </c>
       <c r="D146" t="s">
-        <v>261</v>
+        <v>280</v>
       </c>
     </row>
     <row r="147" spans="1:4">
@@ -2999,7 +2999,7 @@
         <v>149</v>
       </c>
       <c r="B147" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="148" spans="1:4">
@@ -3007,13 +3007,13 @@
         <v>150</v>
       </c>
       <c r="B148" t="s">
+        <v>250</v>
+      </c>
+      <c r="C148" t="s">
         <v>264</v>
       </c>
-      <c r="C148" t="s">
-        <v>247</v>
-      </c>
       <c r="D148" t="s">
-        <v>261</v>
+        <v>280</v>
       </c>
     </row>
     <row r="149" spans="1:4">
@@ -3021,13 +3021,13 @@
         <v>151</v>
       </c>
       <c r="B149" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="C149" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="D149" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
     </row>
     <row r="150" spans="1:4">
@@ -3035,13 +3035,13 @@
         <v>152</v>
       </c>
       <c r="B150" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
       <c r="C150" t="s">
-        <v>269</v>
+        <v>276</v>
       </c>
       <c r="D150" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
     </row>
     <row r="151" spans="1:4">
@@ -3049,13 +3049,13 @@
         <v>153</v>
       </c>
       <c r="B151" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
       <c r="C151" t="s">
+        <v>271</v>
+      </c>
+      <c r="D151" t="s">
         <v>250</v>
-      </c>
-      <c r="D151" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="152" spans="1:4">
@@ -3063,13 +3063,13 @@
         <v>154</v>
       </c>
       <c r="B152" t="s">
-        <v>262</v>
+        <v>248</v>
       </c>
       <c r="C152" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="D152" t="s">
-        <v>280</v>
+        <v>246</v>
       </c>
     </row>
     <row r="153" spans="1:4">
@@ -3077,10 +3077,10 @@
         <v>155</v>
       </c>
       <c r="B153" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="C153" t="s">
-        <v>248</v>
+        <v>266</v>
       </c>
     </row>
     <row r="154" spans="1:4">
@@ -3088,10 +3088,10 @@
         <v>156</v>
       </c>
       <c r="B154" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
       <c r="D154" t="s">
-        <v>248</v>
+        <v>280</v>
       </c>
     </row>
     <row r="155" spans="1:4">
@@ -3099,7 +3099,7 @@
         <v>157</v>
       </c>
       <c r="B155" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
     </row>
     <row r="156" spans="1:4">
@@ -3107,7 +3107,7 @@
         <v>158</v>
       </c>
       <c r="B156" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
     </row>
     <row r="157" spans="1:4">
@@ -3115,7 +3115,7 @@
         <v>159</v>
       </c>
       <c r="B157" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
     </row>
     <row r="158" spans="1:4">
@@ -3123,10 +3123,10 @@
         <v>160</v>
       </c>
       <c r="B158" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="C158" t="s">
-        <v>247</v>
+        <v>258</v>
       </c>
     </row>
     <row r="159" spans="1:4">
@@ -3134,13 +3134,13 @@
         <v>161</v>
       </c>
       <c r="B159" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="C159" t="s">
-        <v>250</v>
+        <v>271</v>
       </c>
       <c r="D159" t="s">
-        <v>281</v>
+        <v>249</v>
       </c>
     </row>
     <row r="160" spans="1:4">
@@ -3148,13 +3148,13 @@
         <v>162</v>
       </c>
       <c r="B160" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="C160" t="s">
+        <v>271</v>
+      </c>
+      <c r="D160" t="s">
         <v>250</v>
-      </c>
-      <c r="D160" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="161" spans="1:4">
@@ -3162,10 +3162,10 @@
         <v>163</v>
       </c>
       <c r="B161" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="C161" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
     </row>
     <row r="162" spans="1:4">
@@ -3176,10 +3176,10 @@
         <v>265</v>
       </c>
       <c r="C162" t="s">
-        <v>252</v>
+        <v>267</v>
       </c>
       <c r="D162" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="163" spans="1:4">
@@ -3190,10 +3190,10 @@
         <v>265</v>
       </c>
       <c r="C163" t="s">
-        <v>278</v>
+        <v>259</v>
       </c>
       <c r="D163" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
     </row>
     <row r="164" spans="1:4">
@@ -3204,7 +3204,7 @@
         <v>265</v>
       </c>
       <c r="C164" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="165" spans="1:4">
@@ -3215,10 +3215,10 @@
         <v>265</v>
       </c>
       <c r="C165" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D165" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
     </row>
     <row r="166" spans="1:4">
@@ -3234,7 +3234,7 @@
         <v>169</v>
       </c>
       <c r="C167" t="s">
-        <v>246</v>
+        <v>258</v>
       </c>
     </row>
     <row r="168" spans="1:4">
@@ -3242,7 +3242,7 @@
         <v>170</v>
       </c>
       <c r="C168" t="s">
-        <v>277</v>
+        <v>264</v>
       </c>
     </row>
     <row r="169" spans="1:4">
@@ -3250,7 +3250,7 @@
         <v>171</v>
       </c>
       <c r="C169" t="s">
-        <v>274</v>
+        <v>247</v>
       </c>
     </row>
     <row r="170" spans="1:4">
@@ -3258,10 +3258,10 @@
         <v>172</v>
       </c>
       <c r="C170" t="s">
-        <v>269</v>
+        <v>247</v>
       </c>
       <c r="D170" t="s">
-        <v>280</v>
+        <v>251</v>
       </c>
     </row>
     <row r="171" spans="1:4">
@@ -3269,7 +3269,7 @@
         <v>173</v>
       </c>
       <c r="C171" t="s">
-        <v>251</v>
+        <v>276</v>
       </c>
     </row>
     <row r="172" spans="1:4">
@@ -3277,7 +3277,7 @@
         <v>174</v>
       </c>
       <c r="C172" t="s">
-        <v>252</v>
+        <v>278</v>
       </c>
     </row>
     <row r="173" spans="1:4">
@@ -3285,7 +3285,7 @@
         <v>175</v>
       </c>
       <c r="C173" t="s">
-        <v>253</v>
+        <v>269</v>
       </c>
     </row>
     <row r="174" spans="1:4">
@@ -3293,7 +3293,7 @@
         <v>176</v>
       </c>
       <c r="C174" t="s">
-        <v>248</v>
+        <v>258</v>
       </c>
     </row>
     <row r="175" spans="1:4">
@@ -3301,7 +3301,7 @@
         <v>177</v>
       </c>
       <c r="C175" t="s">
-        <v>245</v>
+        <v>267</v>
       </c>
     </row>
     <row r="176" spans="1:4">
@@ -3309,7 +3309,7 @@
         <v>178</v>
       </c>
       <c r="C176" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
     </row>
     <row r="177" spans="1:4">
@@ -3317,10 +3317,10 @@
         <v>179</v>
       </c>
       <c r="C177" t="s">
-        <v>277</v>
+        <v>247</v>
       </c>
       <c r="D177" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
     </row>
     <row r="178" spans="1:4">
@@ -3328,7 +3328,7 @@
         <v>180</v>
       </c>
       <c r="C178" t="s">
-        <v>252</v>
+        <v>268</v>
       </c>
     </row>
     <row r="179" spans="1:4">
@@ -3336,10 +3336,10 @@
         <v>181</v>
       </c>
       <c r="C179" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="D179" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="180" spans="1:4">
@@ -3347,7 +3347,7 @@
         <v>182</v>
       </c>
       <c r="C180" t="s">
-        <v>248</v>
+        <v>272</v>
       </c>
     </row>
     <row r="181" spans="1:4">
@@ -3355,10 +3355,10 @@
         <v>183</v>
       </c>
       <c r="C181" t="s">
-        <v>272</v>
+        <v>247</v>
       </c>
       <c r="D181" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
     </row>
     <row r="182" spans="1:4">
@@ -3366,10 +3366,10 @@
         <v>184</v>
       </c>
       <c r="C182" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D182" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
     </row>
     <row r="183" spans="1:4">
@@ -3377,7 +3377,7 @@
         <v>185</v>
       </c>
       <c r="C183" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
     </row>
     <row r="184" spans="1:4">
@@ -3385,7 +3385,7 @@
         <v>186</v>
       </c>
       <c r="C184" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="185" spans="1:4">
@@ -3393,7 +3393,7 @@
         <v>187</v>
       </c>
       <c r="C185" t="s">
-        <v>246</v>
+        <v>264</v>
       </c>
     </row>
     <row r="186" spans="1:4">
@@ -3401,7 +3401,7 @@
         <v>188</v>
       </c>
       <c r="C186" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="187" spans="1:4">
@@ -3409,7 +3409,7 @@
         <v>189</v>
       </c>
       <c r="C187" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="188" spans="1:4">
@@ -3417,10 +3417,10 @@
         <v>190</v>
       </c>
       <c r="C188" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D188" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
     </row>
     <row r="189" spans="1:4">
@@ -3428,7 +3428,7 @@
         <v>191</v>
       </c>
       <c r="C189" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
     </row>
     <row r="190" spans="1:4">
@@ -3436,7 +3436,7 @@
         <v>192</v>
       </c>
       <c r="C190" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="191" spans="1:4">
@@ -3444,7 +3444,7 @@
         <v>193</v>
       </c>
       <c r="C191" t="s">
-        <v>250</v>
+        <v>267</v>
       </c>
     </row>
     <row r="192" spans="1:4">
@@ -3452,10 +3452,10 @@
         <v>194</v>
       </c>
       <c r="C192" t="s">
-        <v>251</v>
+        <v>272</v>
       </c>
       <c r="D192" t="s">
-        <v>281</v>
+        <v>250</v>
       </c>
     </row>
     <row r="193" spans="1:4">
@@ -3463,10 +3463,10 @@
         <v>195</v>
       </c>
       <c r="C193" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="D193" t="s">
-        <v>248</v>
+        <v>281</v>
       </c>
     </row>
     <row r="194" spans="1:4">
@@ -3474,7 +3474,7 @@
         <v>196</v>
       </c>
       <c r="C194" t="s">
-        <v>251</v>
+        <v>268</v>
       </c>
     </row>
     <row r="195" spans="1:4">
@@ -3482,10 +3482,10 @@
         <v>197</v>
       </c>
       <c r="C195" t="s">
-        <v>251</v>
+        <v>269</v>
       </c>
       <c r="D195" t="s">
-        <v>260</v>
+        <v>280</v>
       </c>
     </row>
     <row r="196" spans="1:4">
@@ -3493,10 +3493,10 @@
         <v>198</v>
       </c>
       <c r="C196" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="D196" t="s">
-        <v>281</v>
+        <v>250</v>
       </c>
     </row>
     <row r="197" spans="1:4">
@@ -3504,10 +3504,10 @@
         <v>199</v>
       </c>
       <c r="C197" t="s">
-        <v>246</v>
+        <v>274</v>
       </c>
       <c r="D197" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
     </row>
     <row r="198" spans="1:4">
@@ -3515,7 +3515,7 @@
         <v>200</v>
       </c>
       <c r="C198" t="s">
-        <v>245</v>
+        <v>271</v>
       </c>
     </row>
     <row r="199" spans="1:4">
@@ -3523,10 +3523,10 @@
         <v>201</v>
       </c>
       <c r="C199" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="D199" t="s">
-        <v>281</v>
+        <v>246</v>
       </c>
     </row>
     <row r="200" spans="1:4">
@@ -3534,7 +3534,7 @@
         <v>202</v>
       </c>
       <c r="C200" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="201" spans="1:4">
@@ -3542,10 +3542,10 @@
         <v>203</v>
       </c>
       <c r="C201" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="D201" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="202" spans="1:4">
@@ -3553,7 +3553,7 @@
         <v>204</v>
       </c>
       <c r="C202" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
     </row>
     <row r="203" spans="1:4">
@@ -3561,7 +3561,7 @@
         <v>205</v>
       </c>
       <c r="C203" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="204" spans="1:4">
@@ -3569,10 +3569,10 @@
         <v>206</v>
       </c>
       <c r="C204" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D204" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
     </row>
     <row r="205" spans="1:4">
@@ -3596,7 +3596,7 @@
         <v>209</v>
       </c>
       <c r="C207" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="208" spans="1:4">
@@ -3628,7 +3628,7 @@
         <v>213</v>
       </c>
       <c r="D211" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="212" spans="1:4">
@@ -3636,7 +3636,7 @@
         <v>214</v>
       </c>
       <c r="D212" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="213" spans="1:4">
@@ -3644,7 +3644,7 @@
         <v>215</v>
       </c>
       <c r="D213" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="214" spans="1:4">
@@ -3660,7 +3660,7 @@
         <v>217</v>
       </c>
       <c r="D215" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="216" spans="1:4">
@@ -3692,7 +3692,7 @@
         <v>221</v>
       </c>
       <c r="D219" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="220" spans="1:4">
@@ -3700,7 +3700,7 @@
         <v>222</v>
       </c>
       <c r="D220" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="221" spans="1:4">
@@ -3716,7 +3716,7 @@
         <v>224</v>
       </c>
       <c r="D222" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="223" spans="1:4">
@@ -3724,7 +3724,7 @@
         <v>225</v>
       </c>
       <c r="D223" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="224" spans="1:4">
@@ -3732,7 +3732,7 @@
         <v>226</v>
       </c>
       <c r="D224" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="225" spans="1:4">
@@ -3740,7 +3740,7 @@
         <v>227</v>
       </c>
       <c r="D225" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="226" spans="1:4">
@@ -3748,7 +3748,7 @@
         <v>228</v>
       </c>
       <c r="D226" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
     </row>
     <row r="227" spans="1:4">
@@ -3756,7 +3756,7 @@
         <v>229</v>
       </c>
       <c r="D227" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
     </row>
     <row r="228" spans="1:4">
@@ -3764,7 +3764,7 @@
         <v>230</v>
       </c>
       <c r="D228" t="s">
-        <v>280</v>
+        <v>251</v>
       </c>
     </row>
     <row r="229" spans="1:4">
@@ -3772,7 +3772,7 @@
         <v>231</v>
       </c>
       <c r="D229" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
     </row>
     <row r="230" spans="1:4">
@@ -3780,7 +3780,7 @@
         <v>232</v>
       </c>
       <c r="D230" t="s">
-        <v>281</v>
+        <v>251</v>
       </c>
     </row>
     <row r="231" spans="1:4">
@@ -3788,7 +3788,7 @@
         <v>233</v>
       </c>
       <c r="D231" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="232" spans="1:4">
@@ -3804,7 +3804,7 @@
         <v>235</v>
       </c>
       <c r="D233" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
     </row>
     <row r="234" spans="1:4">
@@ -3812,7 +3812,7 @@
         <v>236</v>
       </c>
       <c r="D234" t="s">
-        <v>245</v>
+        <v>281</v>
       </c>
     </row>
     <row r="235" spans="1:4">
@@ -3820,7 +3820,7 @@
         <v>237</v>
       </c>
       <c r="D235" t="s">
-        <v>259</v>
+        <v>281</v>
       </c>
     </row>
     <row r="236" spans="1:4">
@@ -3828,7 +3828,7 @@
         <v>238</v>
       </c>
       <c r="D236" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
     </row>
     <row r="237" spans="1:4">
@@ -3836,7 +3836,7 @@
         <v>239</v>
       </c>
       <c r="D237" t="s">
-        <v>281</v>
+        <v>249</v>
       </c>
     </row>
     <row r="238" spans="1:4">
@@ -3844,7 +3844,7 @@
         <v>240</v>
       </c>
       <c r="D238" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
     </row>
     <row r="239" spans="1:4">
@@ -3852,7 +3852,7 @@
         <v>241</v>
       </c>
       <c r="D239" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
     </row>
     <row r="240" spans="1:4">
@@ -3860,7 +3860,7 @@
         <v>242</v>
       </c>
       <c r="D240" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
     </row>
     <row r="241" spans="1:4">
@@ -3868,7 +3868,7 @@
         <v>243</v>
       </c>
       <c r="D241" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
     </row>
     <row r="242" spans="1:4">
@@ -3876,7 +3876,7 @@
         <v>244</v>
       </c>
       <c r="D242" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>

</xml_diff>